<commit_message>
update with figures with predicted min and max lines
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756073D6-1E65-424A-93BB-A046322A07DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9C6BC9-C619-4DA2-B540-BE438576B8CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -102,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -111,6 +111,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,36 +809,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -847,9 +818,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Weight</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -874,10 +842,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>raw_data!$A$2:$A$16</c:f>
+              <c:f>raw_data!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>44052.348611111112</c:v>
                 </c:pt>
@@ -922,16 +890,34 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>44045.931944444441</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44053.322916666664</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44053.28402777778</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44055.293749999997</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44054.895138888889</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44054.32708333333</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44053.927777777775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>raw_data!$C$2:$C$16</c:f>
+              <c:f>raw_data!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>74.2</c:v>
                 </c:pt>
@@ -976,6 +962,24 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>76.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>74.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>74.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>76.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>74.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>75.400000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2277,16 +2281,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>592929</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16667</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>252411</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3138,15 +3142,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3174,7 +3179,7 @@
         <v>74.2</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D18" si="0">IF(B2&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D2:D22" si="0">IF(B2&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -3416,6 +3421,66 @@
       <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>AM</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>44055.293749999997</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.29375000000000001</v>
+      </c>
+      <c r="C19">
+        <v>74.5</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>44054.895138888889</v>
+      </c>
+      <c r="B20" s="2">
+        <v>76</v>
+      </c>
+      <c r="C20">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>44054.32708333333</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="C21">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>44053.927777777775</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.9277777777777777</v>
+      </c>
+      <c r="C22">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add slightly better graph and updated data
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9C6BC9-C619-4DA2-B540-BE438576B8CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB03474-2DAF-483E-91FF-3E58DBBCB754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -842,10 +842,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>raw_data!$A$2:$A$26</c:f>
+              <c:f>raw_data!$A$2:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>44052.348611111112</c:v>
                 </c:pt>
@@ -908,16 +908,61 @@
                 </c:pt>
                 <c:pt idx="20" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44053.927777777775</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44061.324305555558</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44061.29583333333</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44060.893055555556</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44060.322222222225</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44060.279861111114</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44059.924305555556</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44059.241666666669</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44059.238888888889</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44058.284722222219</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44057.328472222223</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44057.327777777777</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44057.296527777777</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44056.936805555553</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44056.352083333331</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44055.93472222222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>raw_data!$C$2:$C$26</c:f>
+              <c:f>raw_data!$C$2:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>74.2</c:v>
                 </c:pt>
@@ -980,6 +1025,51 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>75.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>73.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>73.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>74.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>74.7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>74.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>74.7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>74.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>74.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>75.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>75.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>76.900000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3142,10 +3232,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3179,7 +3269,7 @@
         <v>74.2</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D22" si="0">IF(B2&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D2:D37" si="0">IF(B2&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -3479,6 +3569,231 @@
         <v>75.400000000000006</v>
       </c>
       <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>44061.324305555558</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.32361111111111113</v>
+      </c>
+      <c r="C23">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>44061.29583333333</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.29583333333333334</v>
+      </c>
+      <c r="C24">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>44060.893055555556</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.8930555555555556</v>
+      </c>
+      <c r="C25">
+        <v>74.2</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>44060.322222222225</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.32222222222222224</v>
+      </c>
+      <c r="C26">
+        <v>74.5</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>44060.279861111114</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="C27">
+        <v>74.2</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>44059.924305555556</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.9243055555555556</v>
+      </c>
+      <c r="C28">
+        <v>74.8</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>44059.241666666669</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.24166666666666667</v>
+      </c>
+      <c r="C29">
+        <v>74.5</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>44059.238888888889</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.2388888888888889</v>
+      </c>
+      <c r="C30">
+        <v>74.7</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>44058.284722222219</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.28750000000000003</v>
+      </c>
+      <c r="C31">
+        <v>74.7</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>44057.328472222223</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.32847222222222222</v>
+      </c>
+      <c r="C32">
+        <v>74.7</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>44057.327777777777</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.32777777777777778</v>
+      </c>
+      <c r="C33">
+        <v>74.7</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>44057.296527777777</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.29652777777777778</v>
+      </c>
+      <c r="C34">
+        <v>74.7</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>44056.936805555553</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.93680555555555556</v>
+      </c>
+      <c r="C35">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>44056.352083333331</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.3520833333333333</v>
+      </c>
+      <c r="C36">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>44055.93472222222</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.93472222222222223</v>
+      </c>
+      <c r="C37">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="D37" t="str">
         <f t="shared" si="0"/>
         <v>PM</v>
       </c>

</xml_diff>

<commit_message>
update data and code
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB03474-2DAF-483E-91FF-3E58DBBCB754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E65C3B-9FA8-4C0F-A3E9-961DCC08F91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -842,10 +842,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>raw_data!$A$2:$A$41</c:f>
+              <c:f>raw_data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44052.348611111112</c:v>
                 </c:pt>
@@ -953,16 +953,46 @@
                 </c:pt>
                 <c:pt idx="35" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44055.93472222222</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44064.359722222223</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44063.920138888891</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44063.370833333334</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44063.370138888888</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44063.309027777781</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44062.926388888889</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44062.345138888886</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44062.344444444447</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44062.320138888892</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44061.944444444445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>raw_data!$C$2:$C$41</c:f>
+              <c:f>raw_data!$C$2:$C$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>74.2</c:v>
                 </c:pt>
@@ -1070,6 +1100,36 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>76.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>73.8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>74.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>73.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>73.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>73.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>74.8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>75.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3232,10 +3292,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3269,7 +3329,7 @@
         <v>74.2</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D37" si="0">IF(B2&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D2:D41" si="0">IF(B2&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -3795,6 +3855,156 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>44064.359722222223</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="C38">
+        <v>73.8</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>44063.920138888891</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.92013888888888884</v>
+      </c>
+      <c r="C39">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>44063.370833333334</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.37083333333333335</v>
+      </c>
+      <c r="C40">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>44063.370138888888</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="C41">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="D41" t="str">
+        <f>IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>44063.309027777781</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="C42">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="D42" t="str">
+        <f>IF(B42&lt;TIME(12,0,0), "AM", "PM")</f>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>44062.926388888889</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.92638888888888893</v>
+      </c>
+      <c r="C43">
+        <v>75</v>
+      </c>
+      <c r="D43" t="str">
+        <f>IF(B43&lt;TIME(12,0,0), "AM", "PM")</f>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>44062.345138888886</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.34513888888888888</v>
+      </c>
+      <c r="C44">
+        <v>74.5</v>
+      </c>
+      <c r="D44" t="str">
+        <f>IF(B44&lt;TIME(12,0,0), "AM", "PM")</f>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>44062.344444444447</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.3444444444444445</v>
+      </c>
+      <c r="C45">
+        <v>74.8</v>
+      </c>
+      <c r="D45" t="str">
+        <f>IF(B45&lt;TIME(12,0,0), "AM", "PM")</f>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>44062.320138888892</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0.32013888888888892</v>
+      </c>
+      <c r="C46">
+        <v>74.2</v>
+      </c>
+      <c r="D46" t="str">
+        <f>IF(B46&lt;TIME(12,0,0), "AM", "PM")</f>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>44061.944444444445</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.94444444444444453</v>
+      </c>
+      <c r="C47">
+        <v>75.5</v>
+      </c>
+      <c r="D47" t="str">
+        <f>IF(B47&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>PM</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add update to end August
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E65C3B-9FA8-4C0F-A3E9-961DCC08F91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870BDF51-D7F1-4575-AE0A-887C15C7D08D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -3292,10 +3292,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3329,7 +3329,7 @@
         <v>74.2</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D41" si="0">IF(B2&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D2:D40" si="0">IF(B2&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -3914,7 +3914,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f>IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D70" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -3929,7 +3929,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D42" t="str">
-        <f>IF(B42&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" si="1"/>
         <v>AM</v>
       </c>
     </row>
@@ -3944,7 +3944,7 @@
         <v>75</v>
       </c>
       <c r="D43" t="str">
-        <f>IF(B43&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" si="1"/>
         <v>PM</v>
       </c>
     </row>
@@ -3959,7 +3959,7 @@
         <v>74.5</v>
       </c>
       <c r="D44" t="str">
-        <f>IF(B44&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" si="1"/>
         <v>AM</v>
       </c>
     </row>
@@ -3974,7 +3974,7 @@
         <v>74.8</v>
       </c>
       <c r="D45" t="str">
-        <f>IF(B45&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" si="1"/>
         <v>AM</v>
       </c>
     </row>
@@ -3989,7 +3989,7 @@
         <v>74.2</v>
       </c>
       <c r="D46" t="str">
-        <f>IF(B46&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" si="1"/>
         <v>AM</v>
       </c>
     </row>
@@ -4004,8 +4004,353 @@
         <v>75.5</v>
       </c>
       <c r="D47" t="str">
-        <f>IF(B47&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" si="1"/>
         <v>PM</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>44074.318055555559</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.31527777777777777</v>
+      </c>
+      <c r="C48">
+        <v>74</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>44073.915972222225</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.9159722222222223</v>
+      </c>
+      <c r="C49">
+        <v>75</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>44073.457638888889</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.45763888888888887</v>
+      </c>
+      <c r="C50">
+        <v>73.2</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>44073.366666666669</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="C51">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>44072.888888888891</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="C52">
+        <v>75</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>44072.381944444445</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="C53">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>44071.332638888889</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.33263888888888887</v>
+      </c>
+      <c r="C54">
+        <v>73.5</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>44071.311111111114</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="C55">
+        <v>73.5</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>44070.362500000003</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="C56">
+        <v>74.3</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>44069.315972222219</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="C57">
+        <v>73.7</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>44068.905555555553</v>
+      </c>
+      <c r="B58" s="2">
+        <v>0.90555555555555556</v>
+      </c>
+      <c r="C58">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>44068.343055555553</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.3430555555555555</v>
+      </c>
+      <c r="C59">
+        <v>74.2</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>44068.323611111111</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0.32361111111111113</v>
+      </c>
+      <c r="C60">
+        <v>74.2</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>44068.320138888892</v>
+      </c>
+      <c r="B61" s="2">
+        <v>0.32013888888888892</v>
+      </c>
+      <c r="C61">
+        <v>74.2</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>44067.927777777775</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0.9277777777777777</v>
+      </c>
+      <c r="C62">
+        <v>73.7</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>44067.336111111108</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="C63">
+        <v>74.2</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>44067.3125</v>
+      </c>
+      <c r="B64" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="C64">
+        <v>74.2</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>44066.909722222219</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="C65">
+        <v>75.3</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>44066.390277777777</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0.39027777777777778</v>
+      </c>
+      <c r="C66">
+        <v>73.5</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>44064.904861111114</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0.90486111111111101</v>
+      </c>
+      <c r="C67">
+        <v>74.8</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>44064.904166666667</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.90416666666666667</v>
+      </c>
+      <c r="C68">
+        <v>74.8</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>44064.359722222223</v>
+      </c>
+      <c r="B69" s="2">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="C69">
+        <v>73.8</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>44074.370833333334</v>
+      </c>
+      <c r="B70" s="2">
+        <v>0.37083333333333335</v>
+      </c>
+      <c r="C70">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add updates and weekly trend tracker
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870BDF51-D7F1-4575-AE0A-887C15C7D08D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC981FD2-7E50-48AC-A46D-65FEA3AA9CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -3292,10 +3292,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3914,7 +3914,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D70" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D72" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -4349,6 +4349,36 @@
         <v>73.400000000000006</v>
       </c>
       <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>44074.878472222219</v>
+      </c>
+      <c r="B71" s="2">
+        <v>0.87847222222222221</v>
+      </c>
+      <c r="C71">
+        <v>74.7</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>44075.344444444447</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0.3444444444444445</v>
+      </c>
+      <c r="C72">
+        <v>73</v>
+      </c>
+      <c r="D72" t="str">
         <f t="shared" si="1"/>
         <v>AM</v>
       </c>

</xml_diff>

<commit_message>
add update w/ weekly trends and differentiation by regimen
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC981FD2-7E50-48AC-A46D-65FEA3AA9CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17E5C97-1E23-4F1C-B49A-DEC499460553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -842,10 +842,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>raw_data!$A$2:$A$47</c:f>
+              <c:f>raw_data!$A$2:$A$92</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="91"/>
                 <c:pt idx="0">
                   <c:v>44052.348611111112</c:v>
                 </c:pt>
@@ -983,16 +983,118 @@
                 </c:pt>
                 <c:pt idx="45" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44061.944444444445</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44074.318055555559</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44073.915972222225</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44073.457638888889</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44073.366666666669</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44072.888888888891</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44072.381944444445</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44071.332638888889</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44071.311111111114</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44070.362500000003</c:v>
+                </c:pt>
+                <c:pt idx="55" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44069.315972222219</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44068.905555555553</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44068.343055555553</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44068.323611111111</c:v>
+                </c:pt>
+                <c:pt idx="59" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44068.320138888892</c:v>
+                </c:pt>
+                <c:pt idx="60" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44067.927777777775</c:v>
+                </c:pt>
+                <c:pt idx="61" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44067.336111111108</c:v>
+                </c:pt>
+                <c:pt idx="62" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44067.3125</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44066.909722222219</c:v>
+                </c:pt>
+                <c:pt idx="64" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44066.390277777777</c:v>
+                </c:pt>
+                <c:pt idx="65" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44064.904861111114</c:v>
+                </c:pt>
+                <c:pt idx="66" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44064.904166666667</c:v>
+                </c:pt>
+                <c:pt idx="67" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44064.359722222223</c:v>
+                </c:pt>
+                <c:pt idx="68" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44074.370833333334</c:v>
+                </c:pt>
+                <c:pt idx="69" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44074.878472222219</c:v>
+                </c:pt>
+                <c:pt idx="70" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44075.344444444447</c:v>
+                </c:pt>
+                <c:pt idx="71" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44077.402083333334</c:v>
+                </c:pt>
+                <c:pt idx="72" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44077.308333333334</c:v>
+                </c:pt>
+                <c:pt idx="73" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44076.90625</c:v>
+                </c:pt>
+                <c:pt idx="74" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44076.331250000003</c:v>
+                </c:pt>
+                <c:pt idx="75" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44076.277083333334</c:v>
+                </c:pt>
+                <c:pt idx="76" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44075.92083333333</c:v>
+                </c:pt>
+                <c:pt idx="77" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44078.342361111114</c:v>
+                </c:pt>
+                <c:pt idx="78" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44078.313194444447</c:v>
+                </c:pt>
+                <c:pt idx="79" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44077.838888888888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>raw_data!$C$2:$C$47</c:f>
+              <c:f>raw_data!$C$2:$C$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="91"/>
                 <c:pt idx="0">
                   <c:v>74.2</c:v>
                 </c:pt>
@@ -1130,6 +1232,108 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>75.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>74.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>74.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>74.3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>73.7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>74.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>73.7</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>75.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>74.8</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>74.8</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>73.8</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>73.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>74.7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73.8</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>73.3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>73.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>72.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>73.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3292,10 +3496,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3914,7 +4118,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D72" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D81" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -4381,6 +4585,141 @@
       <c r="D72" t="str">
         <f t="shared" si="1"/>
         <v>AM</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <v>44077.402083333334</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0.40208333333333335</v>
+      </c>
+      <c r="C73">
+        <v>73.2</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>44077.308333333334</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0.30833333333333335</v>
+      </c>
+      <c r="C74">
+        <v>73.8</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="6">
+        <v>44076.90625</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="C75">
+        <v>74.2</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>44076.331250000003</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.33124999999999999</v>
+      </c>
+      <c r="C76">
+        <v>73.3</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="6">
+        <v>44076.277083333334</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0.27708333333333335</v>
+      </c>
+      <c r="C77">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>44075.92083333333</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.92083333333333339</v>
+      </c>
+      <c r="C78">
+        <v>74.2</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
+        <v>44078.342361111114</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0.34236111111111112</v>
+      </c>
+      <c r="C79">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>44078.313194444447</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0.31319444444444444</v>
+      </c>
+      <c r="C80">
+        <v>73.5</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
+        <v>44077.838888888888</v>
+      </c>
+      <c r="B81" s="2">
+        <v>0.83888888888888891</v>
+      </c>
+      <c r="C81">
+        <v>73.5</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with disappointing last weekend measurements on first keto week
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17E5C97-1E23-4F1C-B49A-DEC499460553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383787EA-ACEE-4709-B775-56E1B67F270C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1086,6 +1086,33 @@
                 <c:pt idx="79" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44077.838888888888</c:v>
                 </c:pt>
+                <c:pt idx="80" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44081.324305555558</c:v>
+                </c:pt>
+                <c:pt idx="81" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44081.314583333333</c:v>
+                </c:pt>
+                <c:pt idx="82" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44080.918055555558</c:v>
+                </c:pt>
+                <c:pt idx="83" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44080.344444444447</c:v>
+                </c:pt>
+                <c:pt idx="84" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44080.341666666667</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>44079.913888888892</c:v>
+                </c:pt>
+                <c:pt idx="86" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44079.297222222223</c:v>
+                </c:pt>
+                <c:pt idx="87" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44078.893055555556</c:v>
+                </c:pt>
+                <c:pt idx="88" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44078.342361111114</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1334,6 +1361,33 @@
                 </c:pt>
                 <c:pt idx="79">
                   <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>73.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>73.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="85" formatCode="h:mm">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>72.599999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3496,10 +3550,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4118,7 +4172,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D81" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D90" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -4720,6 +4774,141 @@
       <c r="D81" t="str">
         <f t="shared" si="1"/>
         <v>PM</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
+        <v>44081.324305555558</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0.32430555555555557</v>
+      </c>
+      <c r="C82">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <v>44081.314583333333</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.31458333333333333</v>
+      </c>
+      <c r="C83">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>44080.918055555558</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.91805555555555562</v>
+      </c>
+      <c r="C84">
+        <v>74.5</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="6">
+        <v>44080.344444444447</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0.3444444444444445</v>
+      </c>
+      <c r="C85">
+        <v>74</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>44080.341666666667</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.34166666666666662</v>
+      </c>
+      <c r="C86">
+        <v>74.5</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>44079.913888888892</v>
+      </c>
+      <c r="B87" s="2">
+        <v>0.91388888888888886</v>
+      </c>
+      <c r="C87" s="2">
+        <v>74.5</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
+        <v>44079.297222222223</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.29722222222222222</v>
+      </c>
+      <c r="C88">
+        <v>74.5</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="6">
+        <v>44078.893055555556</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.8930555555555556</v>
+      </c>
+      <c r="C89">
+        <v>74.5</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>44078.342361111114</v>
+      </c>
+      <c r="B90" s="2">
+        <v>0.34236111111111112</v>
+      </c>
+      <c r="C90">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update series; attempt and fail at paired GAM
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383787EA-ACEE-4709-B775-56E1B67F270C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82D5674-4F80-42E8-A0DA-8209845D039D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -102,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -112,6 +112,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,10 +843,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>raw_data!$A$2:$A$92</c:f>
+              <c:f>raw_data!$A$2:$A$98</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="91"/>
+                <c:ptCount val="97"/>
                 <c:pt idx="0">
                   <c:v>44052.348611111112</c:v>
                 </c:pt>
@@ -1112,16 +1113,28 @@
                 </c:pt>
                 <c:pt idx="88" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44078.342361111114</c:v>
+                </c:pt>
+                <c:pt idx="89" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44082.34375</c:v>
+                </c:pt>
+                <c:pt idx="90" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44082.343055555553</c:v>
+                </c:pt>
+                <c:pt idx="91" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44081.805555555555</c:v>
+                </c:pt>
+                <c:pt idx="92" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44081.695138888892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>raw_data!$C$2:$C$92</c:f>
+              <c:f>raw_data!$C$2:$C$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="91"/>
+                <c:ptCount val="97"/>
                 <c:pt idx="0">
                   <c:v>74.2</c:v>
                 </c:pt>
@@ -1377,7 +1390,7 @@
                 <c:pt idx="84">
                   <c:v>74.5</c:v>
                 </c:pt>
-                <c:pt idx="85" formatCode="h:mm">
+                <c:pt idx="85" formatCode="0.00">
                   <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="86">
@@ -1388,6 +1401,18 @@
                 </c:pt>
                 <c:pt idx="88">
                   <c:v>72.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>72.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>73.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>73.099999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3550,10 +3575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4172,7 +4197,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D90" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D94" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -4858,7 +4883,7 @@
       <c r="B87" s="2">
         <v>0.91388888888888886</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="7">
         <v>74.5</v>
       </c>
       <c r="D87" t="str">
@@ -4911,8 +4936,69 @@
         <v>AM</v>
       </c>
     </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="6">
+        <v>44082.34375</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0.34375</v>
+      </c>
+      <c r="C91">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="6">
+        <v>44082.343055555553</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.3430555555555555</v>
+      </c>
+      <c r="C92">
+        <v>72.5</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="6">
+        <v>44081.805555555555</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="C93">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>44081.695138888892</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0.69513888888888886</v>
+      </c>
+      <c r="C94">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add lowest points and two-weekly estimates
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82D5674-4F80-42E8-A0DA-8209845D039D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5F87A7-AE1E-43BB-8C2B-17CA6755B366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1126,6 +1126,18 @@
                 <c:pt idx="92" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44081.695138888892</c:v>
                 </c:pt>
+                <c:pt idx="93" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44083.331250000003</c:v>
+                </c:pt>
+                <c:pt idx="94" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44083.329861111109</c:v>
+                </c:pt>
+                <c:pt idx="95" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44083.285416666666</c:v>
+                </c:pt>
+                <c:pt idx="96" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44082.850694444445</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1413,6 +1425,18 @@
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>73.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>72.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>74.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3575,10 +3599,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4197,7 +4221,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D94" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D98" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -4992,6 +5016,66 @@
         <v>73.099999999999994</v>
       </c>
       <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="6">
+        <v>44083.331250000003</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0.33124999999999999</v>
+      </c>
+      <c r="C95">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="6">
+        <v>44083.329861111109</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="C96">
+        <v>73.5</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="6">
+        <v>44083.285416666666</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.28541666666666665</v>
+      </c>
+      <c r="C97">
+        <v>73.5</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="6">
+        <v>44082.850694444445</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0.85069444444444453</v>
+      </c>
+      <c r="C98">
+        <v>74.2</v>
+      </c>
+      <c r="D98" t="str">
         <f t="shared" si="1"/>
         <v>PM</v>
       </c>

</xml_diff>

<commit_message>
add update w new lowest weight
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5F87A7-AE1E-43BB-8C2B-17CA6755B366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4980A0B-4AF9-4493-B640-0F752EE7FF97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -843,10 +843,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>raw_data!$A$2:$A$98</c:f>
+              <c:f>raw_data!$A$2:$A$117</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="97"/>
+                <c:ptCount val="116"/>
                 <c:pt idx="0">
                   <c:v>44052.348611111112</c:v>
                 </c:pt>
@@ -1137,16 +1137,28 @@
                 </c:pt>
                 <c:pt idx="96" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44082.850694444445</c:v>
+                </c:pt>
+                <c:pt idx="97" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44084.370833333334</c:v>
+                </c:pt>
+                <c:pt idx="98" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44084.330555555556</c:v>
+                </c:pt>
+                <c:pt idx="99" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44084.286805555559</c:v>
+                </c:pt>
+                <c:pt idx="100" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44083.911805555559</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>raw_data!$C$2:$C$98</c:f>
+              <c:f>raw_data!$C$2:$C$117</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="97"/>
+                <c:ptCount val="116"/>
                 <c:pt idx="0">
                   <c:v>74.2</c:v>
                 </c:pt>
@@ -1437,6 +1449,18 @@
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>72.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>73.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3599,10 +3623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4221,7 +4245,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D98" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D102" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -5076,6 +5100,66 @@
         <v>74.2</v>
       </c>
       <c r="D98" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="6">
+        <v>44084.370833333334</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.37083333333333335</v>
+      </c>
+      <c r="C99">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="6">
+        <v>44084.330555555556</v>
+      </c>
+      <c r="B100" s="2">
+        <v>0.33055555555555555</v>
+      </c>
+      <c r="C100">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="6">
+        <v>44084.286805555559</v>
+      </c>
+      <c r="B101" s="2">
+        <v>0.28680555555555554</v>
+      </c>
+      <c r="C101">
+        <v>72.5</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="6">
+        <v>44083.911805555559</v>
+      </c>
+      <c r="B102" s="2">
+        <v>0.91180555555555554</v>
+      </c>
+      <c r="C102">
+        <v>73.7</v>
+      </c>
+      <c r="D102" t="str">
         <f t="shared" si="1"/>
         <v>PM</v>
       </c>

</xml_diff>

<commit_message>
update series to new lowest weight; add grey lines linking min (AM) series
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4980A0B-4AF9-4493-B640-0F752EE7FF97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172F923B-076F-4E17-A268-0B9047B3004A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1150,6 +1150,15 @@
                 <c:pt idx="100" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44083.911805555559</c:v>
                 </c:pt>
+                <c:pt idx="101" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44085.392361111109</c:v>
+                </c:pt>
+                <c:pt idx="102" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44085.34097222222</c:v>
+                </c:pt>
+                <c:pt idx="103" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44084.861111111109</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1461,6 +1470,15 @@
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>73.7</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>72.7</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>73.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3623,10 +3641,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4245,7 +4263,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D102" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D105" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -5160,6 +5178,51 @@
         <v>73.7</v>
       </c>
       <c r="D102" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="6">
+        <v>44085.392361111109</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="C103">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="6">
+        <v>44085.34097222222</v>
+      </c>
+      <c r="B104" s="2">
+        <v>0.34097222222222223</v>
+      </c>
+      <c r="C104">
+        <v>72.7</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="6">
+        <v>44084.861111111109</v>
+      </c>
+      <c r="B105" s="2">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="C105">
+        <v>73.2</v>
+      </c>
+      <c r="D105" t="str">
         <f t="shared" si="1"/>
         <v>PM</v>
       </c>

</xml_diff>

<commit_message>
add update to weekend
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172F923B-076F-4E17-A268-0B9047B3004A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8547CE18-DFA3-4951-9FF0-988490831852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1159,6 +1159,27 @@
                 <c:pt idx="103" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44084.861111111109</c:v>
                 </c:pt>
+                <c:pt idx="104" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44087.48333333333</c:v>
+                </c:pt>
+                <c:pt idx="105" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44087.270833333336</c:v>
+                </c:pt>
+                <c:pt idx="106" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44086.877083333333</c:v>
+                </c:pt>
+                <c:pt idx="107" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44086.37777777778</c:v>
+                </c:pt>
+                <c:pt idx="108" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44086.367361111108</c:v>
+                </c:pt>
+                <c:pt idx="109" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44086.366666666669</c:v>
+                </c:pt>
+                <c:pt idx="110" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44086.314583333333</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1479,6 +1500,27 @@
                 </c:pt>
                 <c:pt idx="103">
                   <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>72.3</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>72.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>72.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3403,15 +3445,15 @@
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3419,7 +3461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -3430,7 +3472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>44045</v>
       </c>
@@ -3439,7 +3481,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>44046</v>
       </c>
@@ -3448,7 +3490,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>44047</v>
       </c>
@@ -3459,7 +3501,7 @@
         <v>76.8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>44048</v>
       </c>
@@ -3470,7 +3512,7 @@
         <v>76.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>44049</v>
       </c>
@@ -3481,7 +3523,7 @@
         <v>75.900000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>44050</v>
       </c>
@@ -3492,7 +3534,7 @@
         <v>76.599999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>44051</v>
       </c>
@@ -3503,7 +3545,7 @@
         <v>75.199999999999989</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>44052</v>
       </c>
@@ -3512,7 +3554,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -3520,7 +3562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3534,7 +3576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>44045</v>
       </c>
@@ -3542,7 +3584,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>44046</v>
       </c>
@@ -3550,7 +3592,7 @@
         <v>74.8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>44047</v>
       </c>
@@ -3565,7 +3607,7 @@
         <v>1.2999999999999972</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>44048</v>
       </c>
@@ -3580,7 +3622,7 @@
         <v>1.0999999999999943</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>44049</v>
       </c>
@@ -3595,7 +3637,7 @@
         <v>0.60000000000000853</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>44050</v>
       </c>
@@ -3610,7 +3652,7 @@
         <v>1.3499999999999943</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>44051</v>
       </c>
@@ -3625,7 +3667,7 @@
         <v>0.69999999999998863</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>44052</v>
       </c>
@@ -3641,19 +3683,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3667,7 +3709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>44052.348611111112</v>
       </c>
@@ -3682,7 +3724,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>44051.931250000001</v>
       </c>
@@ -3697,7 +3739,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>44051.405555555553</v>
       </c>
@@ -3712,7 +3754,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>44051.404861111114</v>
       </c>
@@ -3727,7 +3769,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>44050.918749999997</v>
       </c>
@@ -3742,7 +3784,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>44050.348611111112</v>
       </c>
@@ -3757,7 +3799,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>44050.328472222223</v>
       </c>
@@ -3772,7 +3814,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>44049.925000000003</v>
       </c>
@@ -3787,7 +3829,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>44049.320138888892</v>
       </c>
@@ -3802,7 +3844,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>44048.918055555558</v>
       </c>
@@ -3817,7 +3859,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>44048.284722222219</v>
       </c>
@@ -3832,7 +3874,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>44047.920138888891</v>
       </c>
@@ -3847,7 +3889,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>44047.290972222225</v>
       </c>
@@ -3862,7 +3904,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>44046.308333333334</v>
       </c>
@@ -3877,7 +3919,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>44045.931944444441</v>
       </c>
@@ -3892,7 +3934,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>44053.322916666664</v>
       </c>
@@ -3907,7 +3949,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>44053.28402777778</v>
       </c>
@@ -3922,7 +3964,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <v>44055.293749999997</v>
       </c>
@@ -3937,7 +3979,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="6">
         <v>44054.895138888889</v>
       </c>
@@ -3952,7 +3994,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="6">
         <v>44054.32708333333</v>
       </c>
@@ -3967,7 +4009,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="6">
         <v>44053.927777777775</v>
       </c>
@@ -3982,7 +4024,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="6">
         <v>44061.324305555558</v>
       </c>
@@ -3997,7 +4039,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
         <v>44061.29583333333</v>
       </c>
@@ -4012,7 +4054,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <v>44060.893055555556</v>
       </c>
@@ -4027,7 +4069,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
         <v>44060.322222222225</v>
       </c>
@@ -4042,7 +4084,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="6">
         <v>44060.279861111114</v>
       </c>
@@ -4057,7 +4099,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
         <v>44059.924305555556</v>
       </c>
@@ -4072,7 +4114,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="6">
         <v>44059.241666666669</v>
       </c>
@@ -4087,7 +4129,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="6">
         <v>44059.238888888889</v>
       </c>
@@ -4102,7 +4144,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="6">
         <v>44058.284722222219</v>
       </c>
@@ -4117,7 +4159,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="6">
         <v>44057.328472222223</v>
       </c>
@@ -4132,7 +4174,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="6">
         <v>44057.327777777777</v>
       </c>
@@ -4147,7 +4189,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="6">
         <v>44057.296527777777</v>
       </c>
@@ -4162,7 +4204,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="6">
         <v>44056.936805555553</v>
       </c>
@@ -4177,7 +4219,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="6">
         <v>44056.352083333331</v>
       </c>
@@ -4192,7 +4234,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="6">
         <v>44055.93472222222</v>
       </c>
@@ -4207,7 +4249,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="6">
         <v>44064.359722222223</v>
       </c>
@@ -4222,7 +4264,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="6">
         <v>44063.920138888891</v>
       </c>
@@ -4237,7 +4279,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="6">
         <v>44063.370833333334</v>
       </c>
@@ -4252,7 +4294,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="6">
         <v>44063.370138888888</v>
       </c>
@@ -4263,11 +4305,11 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D105" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
-        <v>AM</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D41:D112" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="6">
         <v>44063.309027777781</v>
       </c>
@@ -4282,7 +4324,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="6">
         <v>44062.926388888889</v>
       </c>
@@ -4297,7 +4339,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="6">
         <v>44062.345138888886</v>
       </c>
@@ -4312,7 +4354,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="6">
         <v>44062.344444444447</v>
       </c>
@@ -4327,7 +4369,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="6">
         <v>44062.320138888892</v>
       </c>
@@ -4342,7 +4384,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="6">
         <v>44061.944444444445</v>
       </c>
@@ -4357,7 +4399,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="6">
         <v>44074.318055555559</v>
       </c>
@@ -4372,7 +4414,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="6">
         <v>44073.915972222225</v>
       </c>
@@ -4387,7 +4429,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="6">
         <v>44073.457638888889</v>
       </c>
@@ -4402,7 +4444,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="6">
         <v>44073.366666666669</v>
       </c>
@@ -4417,7 +4459,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="6">
         <v>44072.888888888891</v>
       </c>
@@ -4432,7 +4474,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="6">
         <v>44072.381944444445</v>
       </c>
@@ -4447,7 +4489,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="6">
         <v>44071.332638888889</v>
       </c>
@@ -4462,7 +4504,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="6">
         <v>44071.311111111114</v>
       </c>
@@ -4477,7 +4519,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="6">
         <v>44070.362500000003</v>
       </c>
@@ -4492,7 +4534,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="6">
         <v>44069.315972222219</v>
       </c>
@@ -4507,7 +4549,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="6">
         <v>44068.905555555553</v>
       </c>
@@ -4522,7 +4564,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="6">
         <v>44068.343055555553</v>
       </c>
@@ -4537,7 +4579,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="6">
         <v>44068.323611111111</v>
       </c>
@@ -4552,7 +4594,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="6">
         <v>44068.320138888892</v>
       </c>
@@ -4567,7 +4609,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="6">
         <v>44067.927777777775</v>
       </c>
@@ -4582,7 +4624,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="6">
         <v>44067.336111111108</v>
       </c>
@@ -4597,7 +4639,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="6">
         <v>44067.3125</v>
       </c>
@@ -4612,7 +4654,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="6">
         <v>44066.909722222219</v>
       </c>
@@ -4627,7 +4669,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="6">
         <v>44066.390277777777</v>
       </c>
@@ -4642,7 +4684,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="6">
         <v>44064.904861111114</v>
       </c>
@@ -4657,7 +4699,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="6">
         <v>44064.904166666667</v>
       </c>
@@ -4672,7 +4714,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="6">
         <v>44064.359722222223</v>
       </c>
@@ -4687,7 +4729,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="6">
         <v>44074.370833333334</v>
       </c>
@@ -4702,7 +4744,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="6">
         <v>44074.878472222219</v>
       </c>
@@ -4717,7 +4759,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="6">
         <v>44075.344444444447</v>
       </c>
@@ -4732,7 +4774,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="6">
         <v>44077.402083333334</v>
       </c>
@@ -4747,7 +4789,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="6">
         <v>44077.308333333334</v>
       </c>
@@ -4762,7 +4804,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="6">
         <v>44076.90625</v>
       </c>
@@ -4777,7 +4819,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="6">
         <v>44076.331250000003</v>
       </c>
@@ -4792,7 +4834,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="6">
         <v>44076.277083333334</v>
       </c>
@@ -4807,7 +4849,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="6">
         <v>44075.92083333333</v>
       </c>
@@ -4822,7 +4864,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="6">
         <v>44078.342361111114</v>
       </c>
@@ -4837,7 +4879,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="6">
         <v>44078.313194444447</v>
       </c>
@@ -4852,7 +4894,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="6">
         <v>44077.838888888888</v>
       </c>
@@ -4867,7 +4909,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="6">
         <v>44081.324305555558</v>
       </c>
@@ -4882,7 +4924,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="6">
         <v>44081.314583333333</v>
       </c>
@@ -4897,7 +4939,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" s="6">
         <v>44080.918055555558</v>
       </c>
@@ -4912,7 +4954,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="6">
         <v>44080.344444444447</v>
       </c>
@@ -4927,7 +4969,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" s="6">
         <v>44080.341666666667</v>
       </c>
@@ -4942,7 +4984,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>44079.913888888892</v>
       </c>
@@ -4957,7 +4999,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" s="6">
         <v>44079.297222222223</v>
       </c>
@@ -4972,7 +5014,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" s="6">
         <v>44078.893055555556</v>
       </c>
@@ -4987,7 +5029,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" s="6">
         <v>44078.342361111114</v>
       </c>
@@ -5002,7 +5044,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" s="6">
         <v>44082.34375</v>
       </c>
@@ -5017,7 +5059,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="6">
         <v>44082.343055555553</v>
       </c>
@@ -5032,7 +5074,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="6">
         <v>44081.805555555555</v>
       </c>
@@ -5047,7 +5089,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" s="6">
         <v>44081.695138888892</v>
       </c>
@@ -5062,7 +5104,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" s="6">
         <v>44083.331250000003</v>
       </c>
@@ -5077,7 +5119,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" s="6">
         <v>44083.329861111109</v>
       </c>
@@ -5092,7 +5134,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" s="6">
         <v>44083.285416666666</v>
       </c>
@@ -5107,7 +5149,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" s="6">
         <v>44082.850694444445</v>
       </c>
@@ -5122,7 +5164,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" s="6">
         <v>44084.370833333334</v>
       </c>
@@ -5137,7 +5179,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" s="6">
         <v>44084.330555555556</v>
       </c>
@@ -5152,7 +5194,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" s="6">
         <v>44084.286805555559</v>
       </c>
@@ -5167,7 +5209,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" s="6">
         <v>44083.911805555559</v>
       </c>
@@ -5182,7 +5224,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" s="6">
         <v>44085.392361111109</v>
       </c>
@@ -5197,7 +5239,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" s="6">
         <v>44085.34097222222</v>
       </c>
@@ -5212,7 +5254,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" s="6">
         <v>44084.861111111109</v>
       </c>
@@ -5225,6 +5267,111 @@
       <c r="D105" t="str">
         <f t="shared" si="1"/>
         <v>PM</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A106" s="6">
+        <v>44087.48333333333</v>
+      </c>
+      <c r="B106" s="2">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="C106">
+        <v>72</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A107" s="6">
+        <v>44087.270833333336</v>
+      </c>
+      <c r="B107" s="2">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C107">
+        <v>72.5</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A108" s="6">
+        <v>44086.877083333333</v>
+      </c>
+      <c r="B108" s="2">
+        <v>0.87708333333333333</v>
+      </c>
+      <c r="C108">
+        <v>73.2</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A109" s="6">
+        <v>44086.37777777778</v>
+      </c>
+      <c r="B109" s="2">
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="C109">
+        <v>72.3</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A110" s="6">
+        <v>44086.367361111108</v>
+      </c>
+      <c r="B110" s="2">
+        <v>0.36736111111111108</v>
+      </c>
+      <c r="C110">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A111" s="6">
+        <v>44086.366666666669</v>
+      </c>
+      <c r="B111" s="2">
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="C111">
+        <v>72.5</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A112" s="6">
+        <v>44086.314583333333</v>
+      </c>
+      <c r="B112" s="2">
+        <v>0.31458333333333333</v>
+      </c>
+      <c r="C112">
+        <v>72.5</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add update and adjust position for description box on main figure
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8547CE18-DFA3-4951-9FF0-988490831852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199A86EC-528B-4E0E-AA33-BB2188FE0616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1180,6 +1180,21 @@
                 <c:pt idx="110" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44086.314583333333</c:v>
                 </c:pt>
+                <c:pt idx="111" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44089.36041666667</c:v>
+                </c:pt>
+                <c:pt idx="112" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44089.359722222223</c:v>
+                </c:pt>
+                <c:pt idx="113" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44089.336111111108</c:v>
+                </c:pt>
+                <c:pt idx="114" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44088.879166666666</c:v>
+                </c:pt>
+                <c:pt idx="115" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44088.493750000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1521,6 +1536,21 @@
                 </c:pt>
                 <c:pt idx="110">
                   <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>72.2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>72.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>72.2</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>72.7</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>72.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3445,15 +3475,15 @@
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3461,7 +3491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -3472,7 +3502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>44045</v>
       </c>
@@ -3481,7 +3511,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>44046</v>
       </c>
@@ -3490,7 +3520,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>44047</v>
       </c>
@@ -3501,7 +3531,7 @@
         <v>76.8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>44048</v>
       </c>
@@ -3512,7 +3542,7 @@
         <v>76.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>44049</v>
       </c>
@@ -3523,7 +3553,7 @@
         <v>75.900000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>44050</v>
       </c>
@@ -3534,7 +3564,7 @@
         <v>76.599999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>44051</v>
       </c>
@@ -3545,7 +3575,7 @@
         <v>75.199999999999989</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>44052</v>
       </c>
@@ -3554,7 +3584,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -3562,7 +3592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3576,7 +3606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>44045</v>
       </c>
@@ -3584,7 +3614,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>44046</v>
       </c>
@@ -3592,7 +3622,7 @@
         <v>74.8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>44047</v>
       </c>
@@ -3607,7 +3637,7 @@
         <v>1.2999999999999972</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>44048</v>
       </c>
@@ -3622,7 +3652,7 @@
         <v>1.0999999999999943</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>44049</v>
       </c>
@@ -3637,7 +3667,7 @@
         <v>0.60000000000000853</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>44050</v>
       </c>
@@ -3652,7 +3682,7 @@
         <v>1.3499999999999943</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>44051</v>
       </c>
@@ -3667,7 +3697,7 @@
         <v>0.69999999999998863</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>44052</v>
       </c>
@@ -3683,19 +3713,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3709,7 +3739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44052.348611111112</v>
       </c>
@@ -3724,7 +3754,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44051.931250000001</v>
       </c>
@@ -3739,7 +3769,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44051.405555555553</v>
       </c>
@@ -3754,7 +3784,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44051.404861111114</v>
       </c>
@@ -3769,7 +3799,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44050.918749999997</v>
       </c>
@@ -3784,7 +3814,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44050.348611111112</v>
       </c>
@@ -3799,7 +3829,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44050.328472222223</v>
       </c>
@@ -3814,7 +3844,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44049.925000000003</v>
       </c>
@@ -3829,7 +3859,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44049.320138888892</v>
       </c>
@@ -3844,7 +3874,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44048.918055555558</v>
       </c>
@@ -3859,7 +3889,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44048.284722222219</v>
       </c>
@@ -3874,7 +3904,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44047.920138888891</v>
       </c>
@@ -3889,7 +3919,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44047.290972222225</v>
       </c>
@@ -3904,7 +3934,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44046.308333333334</v>
       </c>
@@ -3919,7 +3949,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44045.931944444441</v>
       </c>
@@ -3934,7 +3964,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44053.322916666664</v>
       </c>
@@ -3949,7 +3979,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44053.28402777778</v>
       </c>
@@ -3964,7 +3994,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>44055.293749999997</v>
       </c>
@@ -3979,7 +4009,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>44054.895138888889</v>
       </c>
@@ -3994,7 +4024,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>44054.32708333333</v>
       </c>
@@ -4009,7 +4039,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>44053.927777777775</v>
       </c>
@@ -4024,7 +4054,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>44061.324305555558</v>
       </c>
@@ -4039,7 +4069,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>44061.29583333333</v>
       </c>
@@ -4054,7 +4084,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>44060.893055555556</v>
       </c>
@@ -4069,7 +4099,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>44060.322222222225</v>
       </c>
@@ -4084,7 +4114,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>44060.279861111114</v>
       </c>
@@ -4099,7 +4129,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>44059.924305555556</v>
       </c>
@@ -4114,7 +4144,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>44059.241666666669</v>
       </c>
@@ -4129,7 +4159,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>44059.238888888889</v>
       </c>
@@ -4144,7 +4174,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>44058.284722222219</v>
       </c>
@@ -4159,7 +4189,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>44057.328472222223</v>
       </c>
@@ -4174,7 +4204,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>44057.327777777777</v>
       </c>
@@ -4189,7 +4219,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>44057.296527777777</v>
       </c>
@@ -4204,7 +4234,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>44056.936805555553</v>
       </c>
@@ -4219,7 +4249,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>44056.352083333331</v>
       </c>
@@ -4234,7 +4264,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>44055.93472222222</v>
       </c>
@@ -4249,7 +4279,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>44064.359722222223</v>
       </c>
@@ -4264,7 +4294,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>44063.920138888891</v>
       </c>
@@ -4279,7 +4309,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>44063.370833333334</v>
       </c>
@@ -4294,7 +4324,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>44063.370138888888</v>
       </c>
@@ -4305,11 +4335,11 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D112" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
-        <v>AM</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+        <f t="shared" ref="D41:D124" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>44063.309027777781</v>
       </c>
@@ -4324,7 +4354,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>44062.926388888889</v>
       </c>
@@ -4339,7 +4369,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>44062.345138888886</v>
       </c>
@@ -4354,7 +4384,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>44062.344444444447</v>
       </c>
@@ -4369,7 +4399,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>44062.320138888892</v>
       </c>
@@ -4384,7 +4414,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>44061.944444444445</v>
       </c>
@@ -4399,7 +4429,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>44074.318055555559</v>
       </c>
@@ -4414,7 +4444,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>44073.915972222225</v>
       </c>
@@ -4429,7 +4459,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>44073.457638888889</v>
       </c>
@@ -4444,7 +4474,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>44073.366666666669</v>
       </c>
@@ -4459,7 +4489,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>44072.888888888891</v>
       </c>
@@ -4474,7 +4504,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>44072.381944444445</v>
       </c>
@@ -4489,7 +4519,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>44071.332638888889</v>
       </c>
@@ -4504,7 +4534,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>44071.311111111114</v>
       </c>
@@ -4519,7 +4549,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>44070.362500000003</v>
       </c>
@@ -4534,7 +4564,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>44069.315972222219</v>
       </c>
@@ -4549,7 +4579,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>44068.905555555553</v>
       </c>
@@ -4564,7 +4594,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>44068.343055555553</v>
       </c>
@@ -4579,7 +4609,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>44068.323611111111</v>
       </c>
@@ -4594,7 +4624,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>44068.320138888892</v>
       </c>
@@ -4609,7 +4639,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>44067.927777777775</v>
       </c>
@@ -4624,7 +4654,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>44067.336111111108</v>
       </c>
@@ -4639,7 +4669,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>44067.3125</v>
       </c>
@@ -4654,7 +4684,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>44066.909722222219</v>
       </c>
@@ -4669,7 +4699,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>44066.390277777777</v>
       </c>
@@ -4684,7 +4714,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>44064.904861111114</v>
       </c>
@@ -4699,7 +4729,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>44064.904166666667</v>
       </c>
@@ -4714,7 +4744,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>44064.359722222223</v>
       </c>
@@ -4729,7 +4759,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>44074.370833333334</v>
       </c>
@@ -4744,7 +4774,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>44074.878472222219</v>
       </c>
@@ -4759,7 +4789,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>44075.344444444447</v>
       </c>
@@ -4774,7 +4804,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>44077.402083333334</v>
       </c>
@@ -4789,7 +4819,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>44077.308333333334</v>
       </c>
@@ -4804,7 +4834,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>44076.90625</v>
       </c>
@@ -4819,7 +4849,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>44076.331250000003</v>
       </c>
@@ -4834,7 +4864,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>44076.277083333334</v>
       </c>
@@ -4849,7 +4879,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>44075.92083333333</v>
       </c>
@@ -4864,7 +4894,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>44078.342361111114</v>
       </c>
@@ -4879,7 +4909,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>44078.313194444447</v>
       </c>
@@ -4894,7 +4924,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>44077.838888888888</v>
       </c>
@@ -4909,7 +4939,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>44081.324305555558</v>
       </c>
@@ -4924,7 +4954,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>44081.314583333333</v>
       </c>
@@ -4939,7 +4969,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <v>44080.918055555558</v>
       </c>
@@ -4954,7 +4984,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
         <v>44080.344444444447</v>
       </c>
@@ -4969,7 +4999,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
         <v>44080.341666666667</v>
       </c>
@@ -4984,7 +5014,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44079.913888888892</v>
       </c>
@@ -4999,7 +5029,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
         <v>44079.297222222223</v>
       </c>
@@ -5014,7 +5044,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="6">
         <v>44078.893055555556</v>
       </c>
@@ -5029,7 +5059,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>44078.342361111114</v>
       </c>
@@ -5044,7 +5074,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
         <v>44082.34375</v>
       </c>
@@ -5059,7 +5089,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>44082.343055555553</v>
       </c>
@@ -5074,7 +5104,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
         <v>44081.805555555555</v>
       </c>
@@ -5089,7 +5119,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>44081.695138888892</v>
       </c>
@@ -5104,7 +5134,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
         <v>44083.331250000003</v>
       </c>
@@ -5119,7 +5149,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
         <v>44083.329861111109</v>
       </c>
@@ -5134,7 +5164,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="6">
         <v>44083.285416666666</v>
       </c>
@@ -5149,7 +5179,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
         <v>44082.850694444445</v>
       </c>
@@ -5164,7 +5194,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
         <v>44084.370833333334</v>
       </c>
@@ -5179,7 +5209,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="6">
         <v>44084.330555555556</v>
       </c>
@@ -5194,7 +5224,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
         <v>44084.286805555559</v>
       </c>
@@ -5209,7 +5239,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>44083.911805555559</v>
       </c>
@@ -5224,7 +5254,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>44085.392361111109</v>
       </c>
@@ -5239,7 +5269,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>44085.34097222222</v>
       </c>
@@ -5254,7 +5284,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
         <v>44084.861111111109</v>
       </c>
@@ -5269,7 +5299,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>44087.48333333333</v>
       </c>
@@ -5284,7 +5314,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="6">
         <v>44087.270833333336</v>
       </c>
@@ -5299,7 +5329,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="6">
         <v>44086.877083333333</v>
       </c>
@@ -5314,7 +5344,7 @@
         <v>PM</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <v>44086.37777777778</v>
       </c>
@@ -5329,7 +5359,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="6">
         <v>44086.367361111108</v>
       </c>
@@ -5344,7 +5374,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="6">
         <v>44086.366666666669</v>
       </c>
@@ -5359,7 +5389,7 @@
         <v>AM</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
         <v>44086.314583333333</v>
       </c>
@@ -5370,6 +5400,186 @@
         <v>72.5</v>
       </c>
       <c r="D112" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="6">
+        <v>44089.36041666667</v>
+      </c>
+      <c r="B113" s="2">
+        <v>0.36041666666666666</v>
+      </c>
+      <c r="C113">
+        <v>72.2</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="6">
+        <v>44089.359722222223</v>
+      </c>
+      <c r="B114" s="2">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="C114">
+        <v>72.2</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="6">
+        <v>44089.336111111108</v>
+      </c>
+      <c r="B115" s="2">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="C115">
+        <v>72.2</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="6">
+        <v>44088.879166666666</v>
+      </c>
+      <c r="B116" s="2">
+        <v>0.87916666666666676</v>
+      </c>
+      <c r="C116">
+        <v>72.7</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="6">
+        <v>44088.493750000001</v>
+      </c>
+      <c r="B117" s="2">
+        <v>0.49374999999999997</v>
+      </c>
+      <c r="C117">
+        <v>72.3</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="6">
+        <v>44088.338888888888</v>
+      </c>
+      <c r="B118" s="2">
+        <v>0.33888888888888885</v>
+      </c>
+      <c r="C118">
+        <v>72.3</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="6">
+        <v>44088.338194444441</v>
+      </c>
+      <c r="B119" s="2">
+        <v>0.33819444444444446</v>
+      </c>
+      <c r="C119">
+        <v>72.8</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="6">
+        <v>44088.308333333334</v>
+      </c>
+      <c r="B120" s="2">
+        <v>0.30833333333333335</v>
+      </c>
+      <c r="C120">
+        <v>72.8</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="6">
+        <v>44088.281944444447</v>
+      </c>
+      <c r="B121" s="2">
+        <v>0.28194444444444444</v>
+      </c>
+      <c r="C121">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="6">
+        <v>44087.922222222223</v>
+      </c>
+      <c r="B122" s="2">
+        <v>0.92222222222222217</v>
+      </c>
+      <c r="C122">
+        <v>73.7</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="6">
+        <v>44087.48333333333</v>
+      </c>
+      <c r="B123" s="2">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="C123">
+        <v>72</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="6">
+        <v>44087.270833333336</v>
+      </c>
+      <c r="B124" s="2">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C124">
+        <v>72.5</v>
+      </c>
+      <c r="D124" t="str">
         <f t="shared" si="1"/>
         <v>AM</v>
       </c>

</xml_diff>

<commit_message>
add dual y axis main fig (weight in stones) + test for weekend effect (not stat sig)
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2E8A5B-B543-4CA8-9210-D1BA65937DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D11972-B347-4CB7-9D86-778E5B7B314A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -843,10 +843,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>raw_data!$A$2:$A$139</c:f>
+              <c:f>raw_data!$A$2:$A$159</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="138"/>
+                <c:ptCount val="158"/>
                 <c:pt idx="0">
                   <c:v>44052.348611111112</c:v>
                 </c:pt>
@@ -1230,16 +1230,31 @@
                 </c:pt>
                 <c:pt idx="127" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44089.890972222223</c:v>
+                </c:pt>
+                <c:pt idx="128" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44091.323611111111</c:v>
+                </c:pt>
+                <c:pt idx="129" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44091.323611111111</c:v>
+                </c:pt>
+                <c:pt idx="130" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44091.310416666667</c:v>
+                </c:pt>
+                <c:pt idx="131" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44081.232638888891</c:v>
+                </c:pt>
+                <c:pt idx="132" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44090.915277777778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>raw_data!$C$2:$C$139</c:f>
+              <c:f>raw_data!$C$2:$C$159</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="138"/>
+                <c:ptCount val="158"/>
                 <c:pt idx="0">
                   <c:v>74.2</c:v>
                 </c:pt>
@@ -1623,6 +1638,21 @@
                 </c:pt>
                 <c:pt idx="127">
                   <c:v>72.2</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>71.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>72.3</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>72.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3785,10 +3815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4407,7 +4437,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D129" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D134" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -5727,6 +5757,81 @@
         <v>72.2</v>
       </c>
       <c r="D129" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="6">
+        <v>44091.323611111111</v>
+      </c>
+      <c r="B130" s="2">
+        <v>0.32361111111111113</v>
+      </c>
+      <c r="C130">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="6">
+        <v>44091.323611111111</v>
+      </c>
+      <c r="B131" s="2">
+        <v>0.32361111111111113</v>
+      </c>
+      <c r="C131">
+        <v>72</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="6">
+        <v>44091.310416666667</v>
+      </c>
+      <c r="B132" s="2">
+        <v>0.31041666666666667</v>
+      </c>
+      <c r="C132">
+        <v>72</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="6">
+        <v>44081.232638888891</v>
+      </c>
+      <c r="B133" s="2">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="C133">
+        <v>72.3</v>
+      </c>
+      <c r="D133" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="6">
+        <v>44090.915277777778</v>
+      </c>
+      <c r="B134" s="2">
+        <v>0.91527777777777775</v>
+      </c>
+      <c r="C134">
+        <v>72.3</v>
+      </c>
+      <c r="D134" t="str">
         <f t="shared" si="1"/>
         <v>PM</v>
       </c>

</xml_diff>

<commit_message>
add new lowest weight; y axis dual axis scale in decistones
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D11972-B347-4CB7-9D86-778E5B7B314A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EED4427-F0BA-484F-AE8C-743F9D7FB29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1246,6 +1246,27 @@
                 <c:pt idx="132" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44090.915277777778</c:v>
                 </c:pt>
+                <c:pt idx="133" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44092.333333333336</c:v>
+                </c:pt>
+                <c:pt idx="134" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44092.333333333336</c:v>
+                </c:pt>
+                <c:pt idx="135" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44092.309027777781</c:v>
+                </c:pt>
+                <c:pt idx="136" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44091.888194444444</c:v>
+                </c:pt>
+                <c:pt idx="137" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44091.352083333331</c:v>
+                </c:pt>
+                <c:pt idx="138" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44091.351388888892</c:v>
+                </c:pt>
+                <c:pt idx="139" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44092.388194444444</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1653,6 +1674,27 @@
                 </c:pt>
                 <c:pt idx="132">
                   <c:v>72.3</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>71.2</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>71.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>72.3</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>71.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>71.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>70.900000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3815,10 +3857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4437,7 +4479,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D134" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D141" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -5834,6 +5876,111 @@
       <c r="D134" t="str">
         <f t="shared" si="1"/>
         <v>PM</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="6">
+        <v>44092.333333333336</v>
+      </c>
+      <c r="B135" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C135">
+        <v>71.2</v>
+      </c>
+      <c r="D135" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="6">
+        <v>44092.333333333336</v>
+      </c>
+      <c r="B136" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C136">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D136" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="6">
+        <v>44092.309027777781</v>
+      </c>
+      <c r="B137" s="2">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="C137">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="D137" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="6">
+        <v>44091.888194444444</v>
+      </c>
+      <c r="B138" s="2">
+        <v>0.8881944444444444</v>
+      </c>
+      <c r="C138">
+        <v>72.3</v>
+      </c>
+      <c r="D138" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="6">
+        <v>44091.352083333331</v>
+      </c>
+      <c r="B139" s="2">
+        <v>0.3520833333333333</v>
+      </c>
+      <c r="C139">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="D139" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="6">
+        <v>44091.351388888892</v>
+      </c>
+      <c r="B140" s="2">
+        <v>0.35138888888888892</v>
+      </c>
+      <c r="C140">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="D140" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="6">
+        <v>44092.388194444444</v>
+      </c>
+      <c r="B141" s="2">
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="C141">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D141" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add projections and update data; add title to date to 69kg graph
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE10282-2AD3-4A9A-816A-446EEC6F8C35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AA471B-F7AF-44FA-B4F6-AB40B5F86897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -843,10 +843,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>raw_data!$A$2:$A$159</c:f>
+              <c:f>raw_data!$A$2:$A$245</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="158"/>
+                <c:ptCount val="244"/>
                 <c:pt idx="0">
                   <c:v>44052.348611111112</c:v>
                 </c:pt>
@@ -1287,16 +1287,34 @@
                 </c:pt>
                 <c:pt idx="146" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44092.925694444442</c:v>
+                </c:pt>
+                <c:pt idx="147" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44095.341666666667</c:v>
+                </c:pt>
+                <c:pt idx="148" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44095.340277777781</c:v>
+                </c:pt>
+                <c:pt idx="149" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44095.306250000001</c:v>
+                </c:pt>
+                <c:pt idx="150" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44094.888888888891</c:v>
+                </c:pt>
+                <c:pt idx="151" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44094.388888888891</c:v>
+                </c:pt>
+                <c:pt idx="152" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44093.897916666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>raw_data!$C$2:$C$159</c:f>
+              <c:f>raw_data!$C$2:$C$245</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="158"/>
+                <c:ptCount val="244"/>
                 <c:pt idx="0">
                   <c:v>74.2</c:v>
                 </c:pt>
@@ -1737,6 +1755,24 @@
                 </c:pt>
                 <c:pt idx="146">
                   <c:v>72.2</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>72.8</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>72.400000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3899,10 +3935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:D154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4521,7 +4557,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D148" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D154" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -6131,7 +6167,94 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="6"/>
+      <c r="A149" s="6">
+        <v>44095.341666666667</v>
+      </c>
+      <c r="B149" s="2">
+        <v>0.34166666666666662</v>
+      </c>
+      <c r="C149">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="6">
+        <v>44095.340277777781</v>
+      </c>
+      <c r="B150" s="2">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C150">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D150" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="6">
+        <v>44095.306250000001</v>
+      </c>
+      <c r="B151" s="2">
+        <v>0.30624999999999997</v>
+      </c>
+      <c r="C151">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D151" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="6">
+        <v>44094.888888888891</v>
+      </c>
+      <c r="B152" s="2">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="C152">
+        <v>72.8</v>
+      </c>
+      <c r="D152" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="6">
+        <v>44094.388888888891</v>
+      </c>
+      <c r="B153" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C153">
+        <v>71.3</v>
+      </c>
+      <c r="D153" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="6">
+        <v>44093.897916666669</v>
+      </c>
+      <c r="B154" s="2">
+        <v>0.8979166666666667</v>
+      </c>
+      <c r="C154">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="D154" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add update to 22/9
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AA471B-F7AF-44FA-B4F6-AB40B5F86897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A46DFE5-60C4-4A65-A3AB-C2F87315C7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1306,6 +1306,27 @@
                 <c:pt idx="152" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44093.897916666669</c:v>
                 </c:pt>
+                <c:pt idx="153" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44096.383333333331</c:v>
+                </c:pt>
+                <c:pt idx="154" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44096.345833333333</c:v>
+                </c:pt>
+                <c:pt idx="155" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44096.331250000003</c:v>
+                </c:pt>
+                <c:pt idx="156" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44095.896527777775</c:v>
+                </c:pt>
+                <c:pt idx="157" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44095.404861111114</c:v>
+                </c:pt>
+                <c:pt idx="158" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44095.404166666667</c:v>
+                </c:pt>
+                <c:pt idx="159" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44095.341666666667</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1773,6 +1794,27 @@
                 </c:pt>
                 <c:pt idx="152">
                   <c:v>72.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>71.2</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>71.7</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>70.8</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>71.099999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3935,10 +3977,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D154"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D217" sqref="D217:D557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4557,7 +4599,7 @@
         <v>73.599999999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D154" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D41:D158" si="1">IF(B41&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -6254,6 +6296,111 @@
       <c r="D154" t="str">
         <f t="shared" si="1"/>
         <v>PM</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="6">
+        <v>44096.383333333331</v>
+      </c>
+      <c r="B155" s="2">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="C155">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="D155" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="6">
+        <v>44096.345833333333</v>
+      </c>
+      <c r="B156" s="2">
+        <v>0.34583333333333338</v>
+      </c>
+      <c r="C156">
+        <v>71.2</v>
+      </c>
+      <c r="D156" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="6">
+        <v>44096.331250000003</v>
+      </c>
+      <c r="B157" s="2">
+        <v>0.33124999999999999</v>
+      </c>
+      <c r="C157">
+        <v>71.7</v>
+      </c>
+      <c r="D157" t="str">
+        <f t="shared" si="1"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="6">
+        <v>44095.896527777775</v>
+      </c>
+      <c r="B158" s="2">
+        <v>0.8965277777777777</v>
+      </c>
+      <c r="C158">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="D158" t="str">
+        <f t="shared" si="1"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="6">
+        <v>44095.404861111114</v>
+      </c>
+      <c r="B159" s="2">
+        <v>0.40486111111111112</v>
+      </c>
+      <c r="C159">
+        <v>70.8</v>
+      </c>
+      <c r="D159" t="str">
+        <f t="shared" ref="D159:D222" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="6">
+        <v>44095.404166666667</v>
+      </c>
+      <c r="B160" s="2">
+        <v>0.40416666666666662</v>
+      </c>
+      <c r="C160">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D160" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="6">
+        <v>44095.341666666667</v>
+      </c>
+      <c r="B161" s="2">
+        <v>0.34166666666666662</v>
+      </c>
+      <c r="C161">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D161" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add update missing pm value yesterday
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A46DFE5-60C4-4A65-A3AB-C2F87315C7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A979B87F-7C16-4A7F-9FD2-94A7582FA144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="15037" yWindow="-1612" windowWidth="21601" windowHeight="11385" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1327,6 +1327,21 @@
                 <c:pt idx="159" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44095.341666666667</c:v>
                 </c:pt>
+                <c:pt idx="160" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44097.324999999997</c:v>
+                </c:pt>
+                <c:pt idx="161" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44097.321527777778</c:v>
+                </c:pt>
+                <c:pt idx="162" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44097.320833333331</c:v>
+                </c:pt>
+                <c:pt idx="163" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44097.320138888892</c:v>
+                </c:pt>
+                <c:pt idx="164" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44096.895833333336</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1815,6 +1830,21 @@
                 </c:pt>
                 <c:pt idx="159">
                   <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>72.099999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3977,10 +4007,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:D166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D217" sqref="D217:D557"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6369,7 +6399,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D222" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D166" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -6401,6 +6431,81 @@
       <c r="D161" t="str">
         <f t="shared" si="2"/>
         <v>AM</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="6">
+        <v>44097.324999999997</v>
+      </c>
+      <c r="B162" s="2">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="C162">
+        <v>71.5</v>
+      </c>
+      <c r="D162" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="6">
+        <v>44097.321527777778</v>
+      </c>
+      <c r="B163" s="2">
+        <v>0.3215277777777778</v>
+      </c>
+      <c r="C163">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="D163" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="6">
+        <v>44097.320833333331</v>
+      </c>
+      <c r="B164" s="2">
+        <v>0.32083333333333336</v>
+      </c>
+      <c r="C164">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="D164" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="6">
+        <v>44097.320138888892</v>
+      </c>
+      <c r="B165" s="2">
+        <v>0.32013888888888892</v>
+      </c>
+      <c r="C165">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="D165" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="6">
+        <v>44096.895833333336</v>
+      </c>
+      <c r="B166" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C166">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="D166" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add update to today; extend back extrapolation period
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A979B87F-7C16-4A7F-9FD2-94A7582FA144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9842BA8-4ACE-4A9B-95C9-19ADCEC4B05D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15037" yWindow="-1612" windowWidth="21601" windowHeight="11385" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1342,6 +1342,18 @@
                 <c:pt idx="164" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44096.895833333336</c:v>
                 </c:pt>
+                <c:pt idx="165" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44098.331250000003</c:v>
+                </c:pt>
+                <c:pt idx="166" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44098.309027777781</c:v>
+                </c:pt>
+                <c:pt idx="167" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44098.308333333334</c:v>
+                </c:pt>
+                <c:pt idx="168" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44097.910416666666</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1845,6 +1857,18 @@
                 </c:pt>
                 <c:pt idx="164">
                   <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>70.8</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>71.8</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>72.400000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4007,10 +4031,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D166"/>
+  <dimension ref="A1:D170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6399,7 +6423,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D166" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D170" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -6504,6 +6528,66 @@
         <v>72.099999999999994</v>
       </c>
       <c r="D166" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="6">
+        <v>44098.331250000003</v>
+      </c>
+      <c r="B167" s="2">
+        <v>0.33124999999999999</v>
+      </c>
+      <c r="C167">
+        <v>70.8</v>
+      </c>
+      <c r="D167" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="6">
+        <v>44098.309027777781</v>
+      </c>
+      <c r="B168" s="2">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="C168">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D168" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="6">
+        <v>44098.308333333334</v>
+      </c>
+      <c r="B169" s="2">
+        <v>0.30833333333333335</v>
+      </c>
+      <c r="C169">
+        <v>71.8</v>
+      </c>
+      <c r="D169" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="6">
+        <v>44097.910416666666</v>
+      </c>
+      <c r="B170" s="2">
+        <v>0.91041666666666676</v>
+      </c>
+      <c r="C170">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="D170" t="str">
         <f t="shared" si="2"/>
         <v>PM</v>
       </c>

</xml_diff>

<commit_message>
update to new lowest weight and slight down creep in projection date
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9842BA8-4ACE-4A9B-95C9-19ADCEC4B05D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC94E3C-6BF0-4250-8028-B50FB0ABC495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1354,6 +1354,27 @@
                 <c:pt idx="168" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44097.910416666666</c:v>
                 </c:pt>
+                <c:pt idx="169" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44099.327777777777</c:v>
+                </c:pt>
+                <c:pt idx="170" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44099.327777777777</c:v>
+                </c:pt>
+                <c:pt idx="171" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44099.302777777775</c:v>
+                </c:pt>
+                <c:pt idx="172" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44099.293055555558</c:v>
+                </c:pt>
+                <c:pt idx="173" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44098.847222222219</c:v>
+                </c:pt>
+                <c:pt idx="174" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44098.361111111109</c:v>
+                </c:pt>
+                <c:pt idx="175" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44098.361111111109</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1869,6 +1890,27 @@
                 </c:pt>
                 <c:pt idx="168">
                   <c:v>72.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>70.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>71.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4031,10 +4073,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D170"/>
+  <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C170" sqref="C170"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6423,7 +6465,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D170" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D177" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -6590,6 +6632,111 @@
       <c r="D170" t="str">
         <f t="shared" si="2"/>
         <v>PM</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="6">
+        <v>44099.327777777777</v>
+      </c>
+      <c r="B171" s="2">
+        <v>0.32777777777777778</v>
+      </c>
+      <c r="C171">
+        <v>70.5</v>
+      </c>
+      <c r="D171" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="6">
+        <v>44099.327777777777</v>
+      </c>
+      <c r="B172" s="2">
+        <v>0.32777777777777778</v>
+      </c>
+      <c r="C172">
+        <v>71</v>
+      </c>
+      <c r="D172" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="6">
+        <v>44099.302777777775</v>
+      </c>
+      <c r="B173" s="2">
+        <v>0.30277777777777776</v>
+      </c>
+      <c r="C173">
+        <v>71</v>
+      </c>
+      <c r="D173" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="6">
+        <v>44099.293055555558</v>
+      </c>
+      <c r="B174" s="2">
+        <v>0.29305555555555557</v>
+      </c>
+      <c r="C174">
+        <v>71</v>
+      </c>
+      <c r="D174" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="6">
+        <v>44098.847222222219</v>
+      </c>
+      <c r="B175" s="2">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="C175">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D175" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="6">
+        <v>44098.361111111109</v>
+      </c>
+      <c r="B176" s="2">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="C176">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D176" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="6">
+        <v>44098.361111111109</v>
+      </c>
+      <c r="B177" s="2">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="C177">
+        <v>71.3</v>
+      </c>
+      <c r="D177" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with strange and disappointing weekend results
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC94E3C-6BF0-4250-8028-B50FB0ABC495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202F13BE-2551-4B36-8997-6346ED358B4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1375,6 +1375,42 @@
                 <c:pt idx="175" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44098.361111111109</c:v>
                 </c:pt>
+                <c:pt idx="176" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44102.357638888891</c:v>
+                </c:pt>
+                <c:pt idx="177" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44102.356944444444</c:v>
+                </c:pt>
+                <c:pt idx="178" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44102.336111111108</c:v>
+                </c:pt>
+                <c:pt idx="179" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.912499999999</c:v>
+                </c:pt>
+                <c:pt idx="180" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.912499999999</c:v>
+                </c:pt>
+                <c:pt idx="181" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.911805555559</c:v>
+                </c:pt>
+                <c:pt idx="182" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.911111111112</c:v>
+                </c:pt>
+                <c:pt idx="183" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.349305555559</c:v>
+                </c:pt>
+                <c:pt idx="184" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.348611111112</c:v>
+                </c:pt>
+                <c:pt idx="185" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.305555555555</c:v>
+                </c:pt>
+                <c:pt idx="186" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.305555555555</c:v>
+                </c:pt>
+                <c:pt idx="187" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44100.340277777781</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1911,6 +1947,42 @@
                 </c:pt>
                 <c:pt idx="175">
                   <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>72.7</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>72.7</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>71.7</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>71.7</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>72.400000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4073,10 +4145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D177"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="A182" sqref="A182"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6465,7 +6537,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D177" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D222" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -6735,6 +6807,186 @@
         <v>71.3</v>
       </c>
       <c r="D177" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="6">
+        <v>44102.357638888891</v>
+      </c>
+      <c r="B178" s="2">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="C178">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D178" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="6">
+        <v>44102.356944444444</v>
+      </c>
+      <c r="B179" s="2">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="C179">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D179" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="6">
+        <v>44102.336111111108</v>
+      </c>
+      <c r="B180" s="2">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="C180">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D180" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="6">
+        <v>44101.912499999999</v>
+      </c>
+      <c r="B181" s="2">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="C181">
+        <v>73.2</v>
+      </c>
+      <c r="D181" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="6">
+        <v>44101.912499999999</v>
+      </c>
+      <c r="B182" s="2">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="C182">
+        <v>73.2</v>
+      </c>
+      <c r="D182" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="6">
+        <v>44101.911805555559</v>
+      </c>
+      <c r="B183" s="2">
+        <v>0.91180555555555554</v>
+      </c>
+      <c r="C183">
+        <v>72.7</v>
+      </c>
+      <c r="D183" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="6">
+        <v>44101.911111111112</v>
+      </c>
+      <c r="B184" s="2">
+        <v>0.91111111111111109</v>
+      </c>
+      <c r="C184">
+        <v>72.7</v>
+      </c>
+      <c r="D184" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="6">
+        <v>44101.349305555559</v>
+      </c>
+      <c r="B185" s="2">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="C185">
+        <v>72</v>
+      </c>
+      <c r="D185" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="6">
+        <v>44101.348611111112</v>
+      </c>
+      <c r="B186" s="2">
+        <v>0.34861111111111115</v>
+      </c>
+      <c r="C186">
+        <v>72</v>
+      </c>
+      <c r="D186" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="6">
+        <v>44101.305555555555</v>
+      </c>
+      <c r="B187" s="2">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="C187">
+        <v>71.7</v>
+      </c>
+      <c r="D187" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="6">
+        <v>44101.305555555555</v>
+      </c>
+      <c r="B188" s="2">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="C188">
+        <v>71.7</v>
+      </c>
+      <c r="D188" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="6">
+        <v>44100.340277777781</v>
+      </c>
+      <c r="B189" s="2">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C189">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="D189" t="str">
         <f t="shared" si="2"/>
         <v>AM</v>
       </c>

</xml_diff>

<commit_message>
update w tues day results (after chips for dinner)
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202F13BE-2551-4B36-8997-6346ED358B4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448D4504-EDD6-488C-BD3D-C7A43A5646F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1411,6 +1411,45 @@
                 <c:pt idx="187" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44100.340277777781</c:v>
                 </c:pt>
+                <c:pt idx="188" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44103.349305555559</c:v>
+                </c:pt>
+                <c:pt idx="189" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44103.332638888889</c:v>
+                </c:pt>
+                <c:pt idx="190" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44103.331944444442</c:v>
+                </c:pt>
+                <c:pt idx="191" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44103.31527777778</c:v>
+                </c:pt>
+                <c:pt idx="192" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44102.357638888891</c:v>
+                </c:pt>
+                <c:pt idx="193" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44102.356944444444</c:v>
+                </c:pt>
+                <c:pt idx="194" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44102.336111111108</c:v>
+                </c:pt>
+                <c:pt idx="195" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.912499999999</c:v>
+                </c:pt>
+                <c:pt idx="196" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44101.911805555559</c:v>
+                </c:pt>
+                <c:pt idx="197" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44104.370138888888</c:v>
+                </c:pt>
+                <c:pt idx="198" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44104.280555555553</c:v>
+                </c:pt>
+                <c:pt idx="199" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44103.884027777778</c:v>
+                </c:pt>
+                <c:pt idx="200" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44103.386805555558</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1983,6 +2022,45 @@
                 </c:pt>
                 <c:pt idx="187">
                   <c:v>72.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>70.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>72.7</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>70.900000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4145,10 +4223,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D189"/>
+  <dimension ref="A1:D202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6537,7 +6615,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D222" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D202" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -6987,6 +7065,201 @@
         <v>72.400000000000006</v>
       </c>
       <c r="D189" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="6">
+        <v>44103.349305555559</v>
+      </c>
+      <c r="B190" s="2">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="C190">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="D190" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="6">
+        <v>44103.332638888889</v>
+      </c>
+      <c r="B191" s="2">
+        <v>0.33263888888888887</v>
+      </c>
+      <c r="C191">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D191" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="6">
+        <v>44103.331944444442</v>
+      </c>
+      <c r="B192" s="2">
+        <v>0.33194444444444443</v>
+      </c>
+      <c r="C192">
+        <v>70.7</v>
+      </c>
+      <c r="D192" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="6">
+        <v>44103.31527777778</v>
+      </c>
+      <c r="B193" s="2">
+        <v>0.31527777777777777</v>
+      </c>
+      <c r="C193">
+        <v>70.7</v>
+      </c>
+      <c r="D193" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="6">
+        <v>44102.357638888891</v>
+      </c>
+      <c r="B194" s="2">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="C194">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D194" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="6">
+        <v>44102.356944444444</v>
+      </c>
+      <c r="B195" s="2">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="C195">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D195" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="6">
+        <v>44102.336111111108</v>
+      </c>
+      <c r="B196" s="2">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="C196">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D196" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="6">
+        <v>44101.912499999999</v>
+      </c>
+      <c r="B197" s="2">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="C197">
+        <v>73.2</v>
+      </c>
+      <c r="D197" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="6">
+        <v>44101.911805555559</v>
+      </c>
+      <c r="B198" s="2">
+        <v>0.91180555555555554</v>
+      </c>
+      <c r="C198">
+        <v>72.7</v>
+      </c>
+      <c r="D198" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="6">
+        <v>44104.370138888888</v>
+      </c>
+      <c r="B199" s="2">
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="C199">
+        <v>71</v>
+      </c>
+      <c r="D199" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="6">
+        <v>44104.280555555553</v>
+      </c>
+      <c r="B200" s="2">
+        <v>0.28055555555555556</v>
+      </c>
+      <c r="C200">
+        <v>71.3</v>
+      </c>
+      <c r="D200" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="6">
+        <v>44103.884027777778</v>
+      </c>
+      <c r="B201" s="2">
+        <v>0.88402777777777775</v>
+      </c>
+      <c r="C201">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D201" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="6">
+        <v>44103.386805555558</v>
+      </c>
+      <c r="B202" s="2">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="C202">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D202" t="str">
         <f t="shared" si="2"/>
         <v>AM</v>
       </c>

</xml_diff>

<commit_message>
add update and fit for projection chart
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448D4504-EDD6-488C-BD3D-C7A43A5646F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBB0185-12B2-4430-B406-B7048B86185A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1450,6 +1450,18 @@
                 <c:pt idx="200" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44103.386805555558</c:v>
                 </c:pt>
+                <c:pt idx="201" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44105.365277777775</c:v>
+                </c:pt>
+                <c:pt idx="202" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44105.364583333336</c:v>
+                </c:pt>
+                <c:pt idx="203" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44105.335416666669</c:v>
+                </c:pt>
+                <c:pt idx="204" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44104.918749999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2061,6 +2073,18 @@
                 </c:pt>
                 <c:pt idx="200">
                   <c:v>70.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>71.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4223,10 +4247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D202"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="B203" sqref="B203"/>
+      <selection activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6615,7 +6639,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D202" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D206" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -7262,6 +7286,66 @@
       <c r="D202" t="str">
         <f t="shared" si="2"/>
         <v>AM</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="6">
+        <v>44105.365277777775</v>
+      </c>
+      <c r="B203" s="2">
+        <v>0.36527777777777781</v>
+      </c>
+      <c r="C203">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D203" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="6">
+        <v>44105.364583333336</v>
+      </c>
+      <c r="B204" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="C204">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D204" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="6">
+        <v>44105.335416666669</v>
+      </c>
+      <c r="B205" s="2">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="C205">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D205" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="6">
+        <v>44104.918749999997</v>
+      </c>
+      <c r="B206" s="2">
+        <v>0.91875000000000007</v>
+      </c>
+      <c r="C206">
+        <v>71.8</v>
+      </c>
+      <c r="D206" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add update to new lowest weight
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655B3591-F0C4-4F29-8EDF-1FB107A9D1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9955061C-FB55-493B-89C2-4874497C7C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -1465,6 +1465,24 @@
                 <c:pt idx="205" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44105.461111111108</c:v>
                 </c:pt>
+                <c:pt idx="206" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44106.379166666666</c:v>
+                </c:pt>
+                <c:pt idx="207" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44106.335416666669</c:v>
+                </c:pt>
+                <c:pt idx="208" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44106.334722222222</c:v>
+                </c:pt>
+                <c:pt idx="209" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44106.30972222222</c:v>
+                </c:pt>
+                <c:pt idx="210" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44106.309027777781</c:v>
+                </c:pt>
+                <c:pt idx="211" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44105.915277777778</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2091,6 +2109,24 @@
                 </c:pt>
                 <c:pt idx="205">
                   <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>71.2</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>71.900000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4253,10 +4289,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="C208" sqref="C208"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="H203" sqref="H203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6645,7 +6681,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D207" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D213" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -7367,6 +7403,96 @@
       <c r="D207" t="str">
         <f t="shared" si="2"/>
         <v>AM</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="6">
+        <v>44106.379166666666</v>
+      </c>
+      <c r="B208" s="2">
+        <v>0.37916666666666665</v>
+      </c>
+      <c r="C208">
+        <v>70</v>
+      </c>
+      <c r="D208" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="6">
+        <v>44106.335416666669</v>
+      </c>
+      <c r="B209" s="2">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="C209">
+        <v>70.7</v>
+      </c>
+      <c r="D209" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="6">
+        <v>44106.334722222222</v>
+      </c>
+      <c r="B210" s="2">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="C210">
+        <v>70.7</v>
+      </c>
+      <c r="D210" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="6">
+        <v>44106.30972222222</v>
+      </c>
+      <c r="B211" s="2">
+        <v>0.30972222222222223</v>
+      </c>
+      <c r="C211">
+        <v>70.7</v>
+      </c>
+      <c r="D211" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="6">
+        <v>44106.309027777781</v>
+      </c>
+      <c r="B212" s="2">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="C212">
+        <v>71.2</v>
+      </c>
+      <c r="D212" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="6">
+        <v>44105.915277777778</v>
+      </c>
+      <c r="B213" s="2">
+        <v>0.91527777777777775</v>
+      </c>
+      <c r="C213">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D213" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ fast data
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9955061C-FB55-493B-89C2-4874497C7C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBA0BAA-E53B-4DFB-B1B3-7F9AFCC7C7A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="15195" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1483,6 +1483,90 @@
                 <c:pt idx="211" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44105.915277777778</c:v>
                 </c:pt>
+                <c:pt idx="212" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44108.425694444442</c:v>
+                </c:pt>
+                <c:pt idx="213" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44108.425694444442</c:v>
+                </c:pt>
+                <c:pt idx="214" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44108.425694444442</c:v>
+                </c:pt>
+                <c:pt idx="215" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44108.367361111108</c:v>
+                </c:pt>
+                <c:pt idx="216" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44108.366666666669</c:v>
+                </c:pt>
+                <c:pt idx="217" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44108.336805555555</c:v>
+                </c:pt>
+                <c:pt idx="218" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44107.932638888888</c:v>
+                </c:pt>
+                <c:pt idx="219" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44107.932638888888</c:v>
+                </c:pt>
+                <c:pt idx="220" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44107.385416666664</c:v>
+                </c:pt>
+                <c:pt idx="221" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44107.384722222225</c:v>
+                </c:pt>
+                <c:pt idx="222" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44107.34097222222</c:v>
+                </c:pt>
+                <c:pt idx="223" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44107.340277777781</c:v>
+                </c:pt>
+                <c:pt idx="224" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44106.881249999999</c:v>
+                </c:pt>
+                <c:pt idx="225" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.317361111112</c:v>
+                </c:pt>
+                <c:pt idx="226" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.316666666666</c:v>
+                </c:pt>
+                <c:pt idx="227" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.272916666669</c:v>
+                </c:pt>
+                <c:pt idx="228" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.148611111108</c:v>
+                </c:pt>
+                <c:pt idx="229" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44109.936111111114</c:v>
+                </c:pt>
+                <c:pt idx="230" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44109.88958333333</c:v>
+                </c:pt>
+                <c:pt idx="231" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44109.729166666664</c:v>
+                </c:pt>
+                <c:pt idx="232" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44109.34097222222</c:v>
+                </c:pt>
+                <c:pt idx="233" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44109.34097222222</c:v>
+                </c:pt>
+                <c:pt idx="234" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44109.306250000001</c:v>
+                </c:pt>
+                <c:pt idx="235" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44109.306250000001</c:v>
+                </c:pt>
+                <c:pt idx="236" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44109.305555555555</c:v>
+                </c:pt>
+                <c:pt idx="237" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44109.292361111111</c:v>
+                </c:pt>
+                <c:pt idx="238" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44108.915972222225</c:v>
+                </c:pt>
+                <c:pt idx="239" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44108.915277777778</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2127,6 +2211,90 @@
                 </c:pt>
                 <c:pt idx="211">
                   <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>69.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>69.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>69.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>69.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>70.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>72.3</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>72.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>71.7</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>72.900000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4289,10 +4457,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D213"/>
+  <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="H203" sqref="H203"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6681,7 +6849,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D213" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D241" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -7491,6 +7659,426 @@
         <v>71.900000000000006</v>
       </c>
       <c r="D213" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="6">
+        <v>44108.425694444442</v>
+      </c>
+      <c r="B214" s="2">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="C214">
+        <v>71.3</v>
+      </c>
+      <c r="D214" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="6">
+        <v>44108.425694444442</v>
+      </c>
+      <c r="B215" s="2">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="C215">
+        <v>71.3</v>
+      </c>
+      <c r="D215" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="6">
+        <v>44108.425694444442</v>
+      </c>
+      <c r="B216" s="2">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="C216">
+        <v>71.3</v>
+      </c>
+      <c r="D216" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="6">
+        <v>44108.367361111108</v>
+      </c>
+      <c r="B217" s="2">
+        <v>0.36736111111111108</v>
+      </c>
+      <c r="C217">
+        <v>71.3</v>
+      </c>
+      <c r="D217" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="6">
+        <v>44108.366666666669</v>
+      </c>
+      <c r="B218" s="2">
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="C218">
+        <v>71.3</v>
+      </c>
+      <c r="D218" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="6">
+        <v>44108.336805555555</v>
+      </c>
+      <c r="B219" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="C219">
+        <v>71.3</v>
+      </c>
+      <c r="D219" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="6">
+        <v>44107.932638888888</v>
+      </c>
+      <c r="B220" s="2">
+        <v>0.93263888888888891</v>
+      </c>
+      <c r="C220">
+        <v>72.5</v>
+      </c>
+      <c r="D220" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="6">
+        <v>44107.932638888888</v>
+      </c>
+      <c r="B221" s="2">
+        <v>0.93263888888888891</v>
+      </c>
+      <c r="C221">
+        <v>72.5</v>
+      </c>
+      <c r="D221" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="6">
+        <v>44107.385416666664</v>
+      </c>
+      <c r="B222" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C222">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D222" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="6">
+        <v>44107.384722222225</v>
+      </c>
+      <c r="B223" s="2">
+        <v>0.38472222222222219</v>
+      </c>
+      <c r="C223">
+        <v>70.7</v>
+      </c>
+      <c r="D223" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="6">
+        <v>44107.34097222222</v>
+      </c>
+      <c r="B224" s="2">
+        <v>0.34097222222222223</v>
+      </c>
+      <c r="C224">
+        <v>70.7</v>
+      </c>
+      <c r="D224" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="6">
+        <v>44107.340277777781</v>
+      </c>
+      <c r="B225" s="2">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C225">
+        <v>70.7</v>
+      </c>
+      <c r="D225" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="6">
+        <v>44106.881249999999</v>
+      </c>
+      <c r="B226" s="2">
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="C226">
+        <v>70.7</v>
+      </c>
+      <c r="D226" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="6">
+        <v>44110.317361111112</v>
+      </c>
+      <c r="B227" s="2">
+        <v>0.31736111111111115</v>
+      </c>
+      <c r="C227">
+        <v>70</v>
+      </c>
+      <c r="D227" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="6">
+        <v>44110.316666666666</v>
+      </c>
+      <c r="B228" s="2">
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="C228">
+        <v>70</v>
+      </c>
+      <c r="D228" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="6">
+        <v>44110.272916666669</v>
+      </c>
+      <c r="B229" s="2">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="C229">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="D229" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="6">
+        <v>44110.148611111108</v>
+      </c>
+      <c r="B230" s="2">
+        <v>0.14861111111111111</v>
+      </c>
+      <c r="C230">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="D230" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="6">
+        <v>44109.936111111114</v>
+      </c>
+      <c r="B231" s="2">
+        <v>0.93611111111111101</v>
+      </c>
+      <c r="C231">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="D231" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="6">
+        <v>44109.88958333333</v>
+      </c>
+      <c r="B232" s="2">
+        <v>0.88958333333333339</v>
+      </c>
+      <c r="C232">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="D232" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="6">
+        <v>44109.729166666664</v>
+      </c>
+      <c r="B233" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C233">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="D233" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="6">
+        <v>44109.34097222222</v>
+      </c>
+      <c r="B234" s="2">
+        <v>0.34097222222222223</v>
+      </c>
+      <c r="C234">
+        <v>72.3</v>
+      </c>
+      <c r="D234" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="6">
+        <v>44109.34097222222</v>
+      </c>
+      <c r="B235" s="2">
+        <v>0.34097222222222223</v>
+      </c>
+      <c r="C235">
+        <v>72</v>
+      </c>
+      <c r="D235" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="6">
+        <v>44109.306250000001</v>
+      </c>
+      <c r="B236" s="2">
+        <v>0.30624999999999997</v>
+      </c>
+      <c r="C236">
+        <v>72</v>
+      </c>
+      <c r="D236" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="6">
+        <v>44109.306250000001</v>
+      </c>
+      <c r="B237" s="2">
+        <v>0.30624999999999997</v>
+      </c>
+      <c r="C237">
+        <v>72</v>
+      </c>
+      <c r="D237" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="6">
+        <v>44109.305555555555</v>
+      </c>
+      <c r="B238" s="2">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="C238">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="D238" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="6">
+        <v>44109.292361111111</v>
+      </c>
+      <c r="B239" s="2">
+        <v>0.29236111111111113</v>
+      </c>
+      <c r="C239">
+        <v>71.7</v>
+      </c>
+      <c r="D239" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="6">
+        <v>44108.915972222225</v>
+      </c>
+      <c r="B240" s="2">
+        <v>0.9159722222222223</v>
+      </c>
+      <c r="C240">
+        <v>72.5</v>
+      </c>
+      <c r="D240" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="6">
+        <v>44108.915277777778</v>
+      </c>
+      <c r="B241" s="2">
+        <v>0.91527777777777775</v>
+      </c>
+      <c r="C241">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D241" t="str">
         <f t="shared" si="2"/>
         <v>PM</v>
       </c>

</xml_diff>

<commit_message>
update after fast and feast week
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBA0BAA-E53B-4DFB-B1B3-7F9AFCC7C7A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E0E3B1-944D-4A1B-8F2A-794A33006C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="15195" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1567,6 +1567,18 @@
                 <c:pt idx="239" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44108.915277777778</c:v>
                 </c:pt>
+                <c:pt idx="240" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44116.344444444447</c:v>
+                </c:pt>
+                <c:pt idx="241" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44116.344444444447</c:v>
+                </c:pt>
+                <c:pt idx="242" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44116.344444444447</c:v>
+                </c:pt>
+                <c:pt idx="243" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44115.414583333331</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2295,6 +2307,18 @@
                 </c:pt>
                 <c:pt idx="239">
                   <c:v>72.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>72.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>72.599999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4457,10 +4481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D241"/>
+  <dimension ref="A1:D268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A242" sqref="A242"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="B269" sqref="B269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6849,7 +6873,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D241" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D268" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -8081,6 +8105,411 @@
       <c r="D241" t="str">
         <f t="shared" si="2"/>
         <v>PM</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="6">
+        <v>44116.344444444447</v>
+      </c>
+      <c r="B242" s="2">
+        <v>0.3444444444444445</v>
+      </c>
+      <c r="C242">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D242" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="6">
+        <v>44116.344444444447</v>
+      </c>
+      <c r="B243" s="2">
+        <v>0.3444444444444445</v>
+      </c>
+      <c r="C243">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D243" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="6">
+        <v>44116.344444444447</v>
+      </c>
+      <c r="B244" s="2">
+        <v>0.3444444444444445</v>
+      </c>
+      <c r="C244">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="D244" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="6">
+        <v>44115.414583333331</v>
+      </c>
+      <c r="B245" s="2">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="C245">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="D245" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="6">
+        <v>44113.370138888888</v>
+      </c>
+      <c r="B246" s="2">
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="C246">
+        <v>71.5</v>
+      </c>
+      <c r="D246" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="6">
+        <v>44113.338194444441</v>
+      </c>
+      <c r="B247" s="2">
+        <v>0.33819444444444446</v>
+      </c>
+      <c r="C247">
+        <v>72</v>
+      </c>
+      <c r="D247" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="6">
+        <v>44112.463888888888</v>
+      </c>
+      <c r="B248" s="2">
+        <v>0.46388888888888885</v>
+      </c>
+      <c r="C248">
+        <v>71</v>
+      </c>
+      <c r="D248" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="6">
+        <v>44112.461805555555</v>
+      </c>
+      <c r="B249" s="2">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="C249">
+        <v>71</v>
+      </c>
+      <c r="D249" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="6">
+        <v>44112.340277777781</v>
+      </c>
+      <c r="B250" s="2">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C250">
+        <v>71</v>
+      </c>
+      <c r="D250" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" s="6">
+        <v>44111.757638888892</v>
+      </c>
+      <c r="B251" s="2">
+        <v>0.75763888888888886</v>
+      </c>
+      <c r="C251">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="D251" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="6">
+        <v>44111.616666666669</v>
+      </c>
+      <c r="B252" s="2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="C252">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="D252" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="6">
+        <v>44111.615972222222</v>
+      </c>
+      <c r="B253" s="2">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="C253">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="D253" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" s="6">
+        <v>44111.474305555559</v>
+      </c>
+      <c r="B254" s="2">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="C254">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="D254" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="6">
+        <v>44111.409722222219</v>
+      </c>
+      <c r="B255" s="2">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C255">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="D255" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="6">
+        <v>44111.40902777778</v>
+      </c>
+      <c r="B256" s="2">
+        <v>0.40902777777777777</v>
+      </c>
+      <c r="C256">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="D256" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="6">
+        <v>44111.408333333333</v>
+      </c>
+      <c r="B257" s="2">
+        <v>0.40833333333333338</v>
+      </c>
+      <c r="C257">
+        <v>71.2</v>
+      </c>
+      <c r="D257" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="6">
+        <v>44111.353472222225</v>
+      </c>
+      <c r="B258" s="2">
+        <v>0.35347222222222219</v>
+      </c>
+      <c r="C258">
+        <v>70</v>
+      </c>
+      <c r="D258" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="6">
+        <v>44111.328472222223</v>
+      </c>
+      <c r="B259" s="2">
+        <v>0.32847222222222222</v>
+      </c>
+      <c r="C259">
+        <v>70.3</v>
+      </c>
+      <c r="D259" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="6">
+        <v>44111.281944444447</v>
+      </c>
+      <c r="B260" s="2">
+        <v>0.28194444444444444</v>
+      </c>
+      <c r="C260">
+        <v>70.3</v>
+      </c>
+      <c r="D260" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="6">
+        <v>44111.276388888888</v>
+      </c>
+      <c r="B261" s="2">
+        <v>0.27638888888888885</v>
+      </c>
+      <c r="C261">
+        <v>70.3</v>
+      </c>
+      <c r="D261" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="6">
+        <v>44111.269444444442</v>
+      </c>
+      <c r="B262" s="2">
+        <v>0.26944444444444443</v>
+      </c>
+      <c r="C262">
+        <v>69.7</v>
+      </c>
+      <c r="D262" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="6">
+        <v>44110.965277777781</v>
+      </c>
+      <c r="B263" s="2">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="C263">
+        <v>70.8</v>
+      </c>
+      <c r="D263" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="6">
+        <v>44110.782638888886</v>
+      </c>
+      <c r="B264" s="2">
+        <v>0.78263888888888899</v>
+      </c>
+      <c r="C264">
+        <v>69.2</v>
+      </c>
+      <c r="D264" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="6">
+        <v>44110.645138888889</v>
+      </c>
+      <c r="B265" s="2">
+        <v>0.64513888888888882</v>
+      </c>
+      <c r="C265">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="D265" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="6">
+        <v>44110.467361111114</v>
+      </c>
+      <c r="B266" s="2">
+        <v>0.46736111111111112</v>
+      </c>
+      <c r="C266">
+        <v>69.2</v>
+      </c>
+      <c r="D266" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" s="6">
+        <v>44110.466666666667</v>
+      </c>
+      <c r="B267" s="2">
+        <v>0.46666666666666662</v>
+      </c>
+      <c r="C267">
+        <v>69.8</v>
+      </c>
+      <c r="D267" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" s="6">
+        <v>44110.380555555559</v>
+      </c>
+      <c r="B268" s="2">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="C268">
+        <v>69.5</v>
+      </c>
+      <c r="D268" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add update to week after rollercoaster week
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E0E3B1-944D-4A1B-8F2A-794A33006C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767C46EC-7445-4FA4-A4C5-675C1D4751F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -4481,10 +4481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D268"/>
+  <dimension ref="A1:D274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="B269" sqref="B269"/>
+    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="A275" sqref="A275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6873,7 +6873,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D268" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D274" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -8508,6 +8508,96 @@
         <v>69.5</v>
       </c>
       <c r="D268" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" s="6">
+        <v>44118.327777777777</v>
+      </c>
+      <c r="B269" s="2">
+        <v>0.32777777777777778</v>
+      </c>
+      <c r="C269">
+        <v>71.3</v>
+      </c>
+      <c r="D269" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="6">
+        <v>44117.92291666667</v>
+      </c>
+      <c r="B270" s="2">
+        <v>0.92291666666666661</v>
+      </c>
+      <c r="C270">
+        <v>71.7</v>
+      </c>
+      <c r="D270" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="6">
+        <v>44117.431944444441</v>
+      </c>
+      <c r="B271" s="2">
+        <v>0.43194444444444446</v>
+      </c>
+      <c r="C271">
+        <v>71.2</v>
+      </c>
+      <c r="D271" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="6">
+        <v>44117.431250000001</v>
+      </c>
+      <c r="B272" s="2">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="C272">
+        <v>71.2</v>
+      </c>
+      <c r="D272" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="6">
+        <v>44117.431250000001</v>
+      </c>
+      <c r="B273" s="2">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="C273">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D273" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="6">
+        <v>44117.334027777775</v>
+      </c>
+      <c r="B274" s="2">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="C274">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D274" t="str">
         <f t="shared" si="2"/>
         <v>AM</v>
       </c>

</xml_diff>

<commit_message>
add projection with weekend effect
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767C46EC-7445-4FA4-A4C5-675C1D4751F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CF5045-84FB-4C1A-9832-8B593AF122B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -4481,10 +4481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D274"/>
+  <dimension ref="A1:D277"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="A275" sqref="A275"/>
+      <selection activeCell="A278" sqref="A278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6873,7 +6873,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D274" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D277" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -8600,6 +8600,51 @@
       <c r="D274" t="str">
         <f t="shared" si="2"/>
         <v>AM</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="6">
+        <v>44119.379861111112</v>
+      </c>
+      <c r="B275" s="2">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="C275">
+        <v>70.5</v>
+      </c>
+      <c r="D275" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="6">
+        <v>44119.325694444444</v>
+      </c>
+      <c r="B276" s="2">
+        <v>0.32569444444444445</v>
+      </c>
+      <c r="C276">
+        <v>70.8</v>
+      </c>
+      <c r="D276" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="6">
+        <v>44118.894444444442</v>
+      </c>
+      <c r="B277" s="2">
+        <v>0.89444444444444438</v>
+      </c>
+      <c r="C277">
+        <v>71.3</v>
+      </c>
+      <c r="D277" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add update 1 day
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CF5045-84FB-4C1A-9832-8B593AF122B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DBBFD1-A587-40C6-B078-CF1DA4D84FCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
+    <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -4481,10 +4481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D277"/>
+  <dimension ref="A1:D283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="A278" sqref="A278"/>
+    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
+      <selection activeCell="C286" sqref="C286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6873,7 +6873,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D277" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D283" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -8645,6 +8645,96 @@
       <c r="D277" t="str">
         <f t="shared" si="2"/>
         <v>PM</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="6">
+        <v>44120.381249999999</v>
+      </c>
+      <c r="B278" s="2">
+        <v>0.38125000000000003</v>
+      </c>
+      <c r="C278">
+        <v>70.5</v>
+      </c>
+      <c r="D278" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="6">
+        <v>44120.380555555559</v>
+      </c>
+      <c r="B279" s="2">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="C279">
+        <v>70.5</v>
+      </c>
+      <c r="D279" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="6">
+        <v>44120.313888888886</v>
+      </c>
+      <c r="B280" s="2">
+        <v>0.31388888888888888</v>
+      </c>
+      <c r="C280">
+        <v>70.5</v>
+      </c>
+      <c r="D280" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" s="6">
+        <v>44119.930555555555</v>
+      </c>
+      <c r="B281" s="2">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="C281">
+        <v>71.2</v>
+      </c>
+      <c r="D281" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="6">
+        <v>44119.379861111112</v>
+      </c>
+      <c r="B282" s="2">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="C282">
+        <v>70.5</v>
+      </c>
+      <c r="D282" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="6">
+        <v>44119.325694444444</v>
+      </c>
+      <c r="B283" s="2">
+        <v>0.32569444444444445</v>
+      </c>
+      <c r="C283">
+        <v>70.8</v>
+      </c>
+      <c r="D283" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add update for weekend
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DBBFD1-A587-40C6-B078-CF1DA4D84FCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C04BD5A-7775-4B88-9CA1-328A501A8835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -4481,10 +4481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D283"/>
+  <dimension ref="A1:D292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="C286" sqref="C286"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A293" sqref="A293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6873,7 +6873,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D283" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D292" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -8735,6 +8735,141 @@
       <c r="D283" t="str">
         <f t="shared" si="2"/>
         <v>AM</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="6">
+        <v>44123.331944444442</v>
+      </c>
+      <c r="B284" s="2">
+        <v>0.33194444444444443</v>
+      </c>
+      <c r="C284">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="D284" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" s="6">
+        <v>44123.331250000003</v>
+      </c>
+      <c r="B285" s="2">
+        <v>0.33124999999999999</v>
+      </c>
+      <c r="C285">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="D285" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" s="6">
+        <v>44123.305555555555</v>
+      </c>
+      <c r="B286" s="2">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="C286">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="D286" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" s="6">
+        <v>44122.356944444444</v>
+      </c>
+      <c r="B287" s="2">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="C287">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="D287" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" s="6">
+        <v>44122.356249999997</v>
+      </c>
+      <c r="B288" s="2">
+        <v>0.35625000000000001</v>
+      </c>
+      <c r="C288">
+        <v>71</v>
+      </c>
+      <c r="D288" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" s="6">
+        <v>44122.355555555558</v>
+      </c>
+      <c r="B289" s="2">
+        <v>0.35555555555555557</v>
+      </c>
+      <c r="C289">
+        <v>71</v>
+      </c>
+      <c r="D289" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="6">
+        <v>44122.293749999997</v>
+      </c>
+      <c r="B290" s="2">
+        <v>0.29375000000000001</v>
+      </c>
+      <c r="C290">
+        <v>71</v>
+      </c>
+      <c r="D290" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="6">
+        <v>44121.300694444442</v>
+      </c>
+      <c r="B291" s="2">
+        <v>0.30069444444444443</v>
+      </c>
+      <c r="C291">
+        <v>71</v>
+      </c>
+      <c r="D291" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="6">
+        <v>44120.928472222222</v>
+      </c>
+      <c r="B292" s="2">
+        <v>0.92847222222222225</v>
+      </c>
+      <c r="C292">
+        <v>71.5</v>
+      </c>
+      <c r="D292" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add update to tues
</commit_message>
<xml_diff>
--- a/weight_over_time.xlsx
+++ b/weight_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Minton\repos\weight_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C04BD5A-7775-4B88-9CA1-328A501A8835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8FFCA9-0F1E-40F9-B66D-94B0559A4C1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-2512" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{0E46FC83-6B64-42C1-BCEB-3F339E81E359}"/>
   </bookViews>
@@ -843,10 +843,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>raw_data!$A$2:$A$245</c:f>
+              <c:f>raw_data!$A$2:$A$501</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="244"/>
+                <c:ptCount val="500"/>
                 <c:pt idx="0">
                   <c:v>44052.348611111112</c:v>
                 </c:pt>
@@ -1578,16 +1578,175 @@
                 </c:pt>
                 <c:pt idx="243" formatCode="m/d/yyyy\ h:mm">
                   <c:v>44115.414583333331</c:v>
+                </c:pt>
+                <c:pt idx="244" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44113.370138888888</c:v>
+                </c:pt>
+                <c:pt idx="245" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44113.338194444441</c:v>
+                </c:pt>
+                <c:pt idx="246" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44112.463888888888</c:v>
+                </c:pt>
+                <c:pt idx="247" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44112.461805555555</c:v>
+                </c:pt>
+                <c:pt idx="248" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44112.340277777781</c:v>
+                </c:pt>
+                <c:pt idx="249" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.757638888892</c:v>
+                </c:pt>
+                <c:pt idx="250" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.616666666669</c:v>
+                </c:pt>
+                <c:pt idx="251" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.615972222222</c:v>
+                </c:pt>
+                <c:pt idx="252" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.474305555559</c:v>
+                </c:pt>
+                <c:pt idx="253" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.409722222219</c:v>
+                </c:pt>
+                <c:pt idx="254" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.40902777778</c:v>
+                </c:pt>
+                <c:pt idx="255" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.408333333333</c:v>
+                </c:pt>
+                <c:pt idx="256" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.353472222225</c:v>
+                </c:pt>
+                <c:pt idx="257" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.328472222223</c:v>
+                </c:pt>
+                <c:pt idx="258" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.281944444447</c:v>
+                </c:pt>
+                <c:pt idx="259" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.276388888888</c:v>
+                </c:pt>
+                <c:pt idx="260" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44111.269444444442</c:v>
+                </c:pt>
+                <c:pt idx="261" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.965277777781</c:v>
+                </c:pt>
+                <c:pt idx="262" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.782638888886</c:v>
+                </c:pt>
+                <c:pt idx="263" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.645138888889</c:v>
+                </c:pt>
+                <c:pt idx="264" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.467361111114</c:v>
+                </c:pt>
+                <c:pt idx="265" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.466666666667</c:v>
+                </c:pt>
+                <c:pt idx="266" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44110.380555555559</c:v>
+                </c:pt>
+                <c:pt idx="267" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44118.327777777777</c:v>
+                </c:pt>
+                <c:pt idx="268" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44117.92291666667</c:v>
+                </c:pt>
+                <c:pt idx="269" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44117.431944444441</c:v>
+                </c:pt>
+                <c:pt idx="270" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44117.431250000001</c:v>
+                </c:pt>
+                <c:pt idx="271" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44117.431250000001</c:v>
+                </c:pt>
+                <c:pt idx="272" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44117.334027777775</c:v>
+                </c:pt>
+                <c:pt idx="273" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44119.379861111112</c:v>
+                </c:pt>
+                <c:pt idx="274" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44119.325694444444</c:v>
+                </c:pt>
+                <c:pt idx="275" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44118.894444444442</c:v>
+                </c:pt>
+                <c:pt idx="276" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44120.381249999999</c:v>
+                </c:pt>
+                <c:pt idx="277" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44120.380555555559</c:v>
+                </c:pt>
+                <c:pt idx="278" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44120.313888888886</c:v>
+                </c:pt>
+                <c:pt idx="279" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44119.930555555555</c:v>
+                </c:pt>
+                <c:pt idx="280" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44119.379861111112</c:v>
+                </c:pt>
+                <c:pt idx="281" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44119.325694444444</c:v>
+                </c:pt>
+                <c:pt idx="282" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44123.331944444442</c:v>
+                </c:pt>
+                <c:pt idx="283" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44123.331250000003</c:v>
+                </c:pt>
+                <c:pt idx="284" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44123.305555555555</c:v>
+                </c:pt>
+                <c:pt idx="285" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44122.356944444444</c:v>
+                </c:pt>
+                <c:pt idx="286" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44122.356249999997</c:v>
+                </c:pt>
+                <c:pt idx="287" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44122.355555555558</c:v>
+                </c:pt>
+                <c:pt idx="288" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44122.293749999997</c:v>
+                </c:pt>
+                <c:pt idx="289" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44121.300694444442</c:v>
+                </c:pt>
+                <c:pt idx="290" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44120.928472222222</c:v>
+                </c:pt>
+                <c:pt idx="291" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44124.363888888889</c:v>
+                </c:pt>
+                <c:pt idx="292" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44124.32708333333</c:v>
+                </c:pt>
+                <c:pt idx="293" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44124.326388888891</c:v>
+                </c:pt>
+                <c:pt idx="294" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44124.326388888891</c:v>
+                </c:pt>
+                <c:pt idx="295" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44124.325694444444</c:v>
+                </c:pt>
+                <c:pt idx="296" formatCode="m/d/yyyy\ h:mm">
+                  <c:v>44123.928472222222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>raw_data!$C$2:$C$245</c:f>
+              <c:f>raw_data!$C$2:$C$501</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="244"/>
+                <c:ptCount val="500"/>
                 <c:pt idx="0">
                   <c:v>74.2</c:v>
                 </c:pt>
@@ -2319,6 +2478,165 @@
                 </c:pt>
                 <c:pt idx="243">
                   <c:v>72.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>69.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>69.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>69.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>70.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>70.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>70.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>71.2</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>70.3</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>70.3</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>70.3</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>69.7</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>70.8</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>69.2</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>69.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>69.2</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>69.8</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>69.5</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>71.7</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>71.2</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>71.2</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>70.8</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>71.2</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>70.8</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>70.2</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>70.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>70.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>70.599999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4481,10 +4799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF6914-47A5-43B9-B1AB-1012335C7F10}">
-  <dimension ref="A1:D292"/>
+  <dimension ref="A1:D298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A293" sqref="A293"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="A299" sqref="A299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6873,7 +7191,7 @@
         <v>70.8</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" ref="D159:D292" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
+        <f t="shared" ref="D159:D298" si="2">IF(B159&lt;TIME(12,0,0), "AM", "PM")</f>
         <v>AM</v>
       </c>
     </row>
@@ -8868,6 +9186,96 @@
         <v>71.5</v>
       </c>
       <c r="D292" t="str">
+        <f t="shared" si="2"/>
+        <v>PM</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="6">
+        <v>44124.363888888889</v>
+      </c>
+      <c r="B293" s="2">
+        <v>0.36388888888888887</v>
+      </c>
+      <c r="C293">
+        <v>70.2</v>
+      </c>
+      <c r="D293" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="6">
+        <v>44124.32708333333</v>
+      </c>
+      <c r="B294" s="2">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="C294">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D294" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="6">
+        <v>44124.326388888891</v>
+      </c>
+      <c r="B295" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C295">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="D295" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="6">
+        <v>44124.326388888891</v>
+      </c>
+      <c r="B296" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C296">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D296" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" s="6">
+        <v>44124.325694444444</v>
+      </c>
+      <c r="B297" s="2">
+        <v>0.32569444444444445</v>
+      </c>
+      <c r="C297">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D297" t="str">
+        <f t="shared" si="2"/>
+        <v>AM</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="6">
+        <v>44123.928472222222</v>
+      </c>
+      <c r="B298" s="2">
+        <v>0.92847222222222225</v>
+      </c>
+      <c r="C298">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="D298" t="str">
         <f t="shared" si="2"/>
         <v>PM</v>
       </c>

</xml_diff>